<commit_message>
add diagram to tolerances. add RC filter after boosts. sim with PWL
</commit_message>
<xml_diff>
--- a/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
+++ b/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\0 Documentation\1 Design Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B4A897-3FDA-48EC-871B-88D5F5D520A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F2F73B-A639-4E87-909B-FC53C3A731D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" tabRatio="766" firstSheet="1" activeTab="3" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="3" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="6" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="238">
   <si>
     <t>Digital Input Protection</t>
   </si>
@@ -410,24 +410,6 @@
     <t>Tolerance</t>
   </si>
   <si>
-    <t>ADC ENOB</t>
-  </si>
-  <si>
-    <t>Number of LSBs deviation due to VREF tolerance</t>
-  </si>
-  <si>
-    <t>Max-min</t>
-  </si>
-  <si>
-    <t>Log base 2</t>
-  </si>
-  <si>
-    <t>Actual ENOB after considering VREF noise</t>
-  </si>
-  <si>
-    <t>VREF / 2^12</t>
-  </si>
-  <si>
     <t>Vref</t>
   </si>
   <si>
@@ -437,9 +419,6 @@
     <t>V/LSB</t>
   </si>
   <si>
-    <t>&lt;-- not valid. Each step will be off by VREF (erroneous) / 2^ENOB</t>
-  </si>
-  <si>
     <t>Non-inverting amplifier Rf</t>
   </si>
   <si>
@@ -813,18 +792,47 @@
   </si>
   <si>
     <t>So theoretically we can hit 1Msps if Teensy is fast enough</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>VREF / 2^ENOB</t>
+  </si>
+  <si>
+    <t>Analog mux: Vishay DG409</t>
+  </si>
+  <si>
+    <t>max gain to keep output voltage within ADC Vref</t>
+  </si>
+  <si>
+    <t>ADC effective number of bits (ENOB)</t>
+  </si>
+  <si>
+    <t>- MCP33131-10-E/MS</t>
+  </si>
+  <si>
+    <t>16-bit SRAR 1Msps SPI single-ended</t>
+  </si>
+  <si>
+    <t>MCP33151 14-bit</t>
+  </si>
+  <si>
+    <t>MCP33131 16-bit</t>
+  </si>
+  <si>
+    <t>Options</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="##0.00E+0"/>
-    <numFmt numFmtId="168" formatCode="##0.000E+0"/>
+    <numFmt numFmtId="166" formatCode="##0.00E+0"/>
+    <numFmt numFmtId="167" formatCode="##0.000E+0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1181,7 +1189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1192,7 +1200,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1254,6 +1261,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1262,18 +1311,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1311,36 +1348,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2499,7 +2506,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>530716</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>111538</xdr:rowOff>
+      <xdr:rowOff>74380</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2546,15 +2553,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>587829</xdr:colOff>
+      <xdr:colOff>591639</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>348343</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>21772</xdr:rowOff>
+      <xdr:colOff>350248</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>20483</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2569,8 +2576,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13530943" y="4604657"/>
-          <a:ext cx="2808514" cy="1240972"/>
+          <a:off x="13588655" y="4603134"/>
+          <a:ext cx="2831190" cy="1808317"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2621,7 +2628,16 @@
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
             <a:t>Will proceed with design as if they do not exist.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
+            <a:t>Teensy 4.0/4.1 pins are all 3.3v only without overvoltage protection.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2676,6 +2692,66 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
+      <xdr:colOff>45719</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11779</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>444730</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>4293</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB913A7-53DA-9C77-4D43-9D06125F2DA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10492739" y="5947759"/>
+          <a:ext cx="3447011" cy="2552834"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>257863</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>133375</xdr:rowOff>
@@ -2722,10 +2798,85 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>37428</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>72951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2868706</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>82252</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D5720A8-975B-3436-B5F1-F79F68EAB6C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3802604" y="3972598"/>
+          <a:ext cx="2831278" cy="1286772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Go</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> with 4.7uH for now, check performance once sample is received. May tune inductor value after receiving the boards.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3078,16 +3229,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5AE85C-D239-4D24-ADF0-BC89AC6A16C4}">
   <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="97" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="16" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
@@ -3096,406 +3247,406 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="K4" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="N4" s="29" t="s">
-        <v>122</v>
+      <c r="C4" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="K4" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="B5" s="62"/>
       <c r="C5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="17">
+        <v>149</v>
+      </c>
+      <c r="E5" s="16">
         <v>0.36499999999999999</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>10</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="27">
         <v>75</v>
       </c>
       <c r="K5" t="str">
         <f>B4</f>
         <v>+5V</v>
       </c>
-      <c r="L5" s="35">
+      <c r="L5" s="34">
         <f>E22</f>
         <v>280.11786000000001</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="34">
         <f>F22</f>
         <v>296.52199999999999</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="34">
         <f>G22</f>
         <v>452.2045</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+      <c r="B6" s="62"/>
       <c r="C6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="28"/>
+        <v>128</v>
+      </c>
+      <c r="G6" s="27"/>
       <c r="K6" t="str">
         <f>B24</f>
         <v>+3V3</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="34">
         <f>E37</f>
         <v>2.8528599999999997</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="34">
         <f t="shared" ref="M6:N6" si="0">F37</f>
         <v>9.0220000000000002</v>
       </c>
-      <c r="N6" s="35">
+      <c r="N6" s="34">
         <f t="shared" si="0"/>
         <v>11.067</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="39"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="17">
+        <v>144</v>
+      </c>
+      <c r="E7" s="16">
         <v>2</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>2</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="27">
         <v>3</v>
       </c>
       <c r="K7" t="str">
         <f>B39</f>
         <v>+12V</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="34">
         <f>E52</f>
         <v>46.64</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="34">
         <f t="shared" ref="M7:N7" si="1">F52</f>
         <v>46.800000000000004</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="34">
         <f t="shared" si="1"/>
         <v>70.17</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
+      <c r="B8" s="62"/>
       <c r="C8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="17">
+        <v>155</v>
+      </c>
+      <c r="E8" s="16">
         <v>100</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>100</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>100</v>
       </c>
       <c r="K8" t="str">
         <f>B54</f>
         <v>-12V</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="34">
         <f>E65</f>
         <v>3.504</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="34">
         <f t="shared" ref="M8:N8" si="2">F65</f>
         <v>4.8</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="34">
         <f t="shared" si="2"/>
         <v>5.8</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="39"/>
-      <c r="G9" s="28"/>
+      <c r="B9" s="62"/>
+      <c r="G9" s="27"/>
       <c r="K9" t="str">
         <f>B67</f>
         <v>+5V_A</v>
       </c>
-      <c r="L9" s="35">
+      <c r="L9" s="34">
         <f>E77</f>
         <v>2.0001199999999999</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="34">
         <f>F77</f>
         <v>2.66</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="34">
         <f>G77</f>
         <v>3.87</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
-      <c r="G10" s="28"/>
+      <c r="B10" s="62"/>
+      <c r="G10" s="27"/>
       <c r="K10" t="str">
         <f>B79</f>
         <v>+1V8_A</v>
       </c>
-      <c r="L10" s="35">
+      <c r="L10" s="34">
         <f>E83</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="34">
         <f>F83</f>
         <v>1.98</v>
       </c>
-      <c r="N10" s="35">
+      <c r="N10" s="34">
         <f>G83</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="39"/>
-      <c r="C11" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="39"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="9"/>
       <c r="E12"/>
       <c r="F12"/>
-      <c r="G12" s="37"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="39"/>
-      <c r="G13" s="28"/>
+      <c r="B13" s="62"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="39"/>
-      <c r="G14" s="28"/>
+      <c r="B14" s="62"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="39"/>
-      <c r="G15" s="28"/>
+      <c r="B15" s="62"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="39"/>
-      <c r="G16" s="28"/>
+      <c r="B16" s="62"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="39"/>
-      <c r="C17" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="39"/>
+      <c r="B18" s="62"/>
       <c r="C18" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" s="17" cm="1">
+        <v>140</v>
+      </c>
+      <c r="E18" s="16" cm="1">
         <f t="array" ref="E18">E52*15/_RAIL_5V/EFF_12V_BOOST</f>
         <v>174.9</v>
       </c>
-      <c r="F18" s="17" cm="1">
+      <c r="F18" s="16" cm="1">
         <f t="array" ref="F18">F52*15/_RAIL_5V/EFF_12V_BOOST</f>
         <v>175.50000000000003</v>
       </c>
-      <c r="G18" s="28" cm="1">
+      <c r="G18" s="27" cm="1">
         <f t="array" ref="G18">G52*15/_RAIL_5V/EFF_12V_BOOST</f>
         <v>263.13749999999999</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="39"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" s="17">
+        <v>142</v>
+      </c>
+      <c r="E19" s="16">
         <f>E37</f>
         <v>2.8528599999999997</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="16">
         <f>F37</f>
         <v>9.0220000000000002</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="27">
         <f>G37</f>
         <v>11.067</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="39"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="9"/>
-      <c r="G20" s="28"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="39"/>
+      <c r="B21" s="62"/>
       <c r="C21" s="9"/>
-      <c r="G21" s="28"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="40"/>
-      <c r="C22" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="31">
+      <c r="B22" s="63"/>
+      <c r="C22" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="30">
         <f>SUM(E5:E20)</f>
         <v>280.11786000000001</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="30">
         <f>SUM(F5:F20)</f>
         <v>296.52199999999999</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="31">
         <f>SUM(G5:G20)</f>
         <v>452.2045</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
+      <c r="C24" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="39"/>
+      <c r="B25" s="62"/>
       <c r="C25" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="17">
+        <v>135</v>
+      </c>
+      <c r="E25" s="16">
         <f>3*0.00012</f>
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="16">
         <f>3*0.4</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="G25" s="28">
+      <c r="G25" s="27">
         <f>3*0.5</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="39"/>
+      <c r="B26" s="62"/>
       <c r="C26" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="17">
+        <v>138</v>
+      </c>
+      <c r="E26" s="16">
         <f>3*0.002</f>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="16">
         <f>G26</f>
         <v>3</v>
       </c>
-      <c r="G26" s="28">
+      <c r="G26" s="27">
         <f>3*1</f>
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="39"/>
+      <c r="B27" s="62"/>
       <c r="C27" t="s">
-        <v>146</v>
-      </c>
-      <c r="E27" s="17">
+        <v>139</v>
+      </c>
+      <c r="E27" s="16">
         <f>24*3.3/100000*1000</f>
         <v>0.79199999999999982</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="16">
         <f>24*3.3/100000*1000</f>
         <v>0.79199999999999982</v>
       </c>
-      <c r="G27" s="28">
+      <c r="G27" s="27">
         <f>24*3.3/100000*1000</f>
         <v>0.79199999999999982</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="39"/>
+      <c r="B28" s="62"/>
       <c r="C28" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="16">
+        <v>2</v>
+      </c>
+      <c r="F28" s="16">
+        <v>2</v>
+      </c>
+      <c r="G28" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="62"/>
+      <c r="C29" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="E28" s="17">
-        <v>2</v>
-      </c>
-      <c r="F28" s="17">
-        <v>2</v>
-      </c>
-      <c r="G28" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="39"/>
-      <c r="C29" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="E29">
         <v>0.05</v>
@@ -3508,526 +3659,526 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="39"/>
-      <c r="G30" s="28"/>
+      <c r="B30" s="62"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="39"/>
-      <c r="G31" s="28"/>
+      <c r="B31" s="62"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="39"/>
-      <c r="G32" s="28"/>
+      <c r="B32" s="62"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="39"/>
-      <c r="C33" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="39"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="17">
+        <v>143</v>
+      </c>
+      <c r="E34" s="16">
         <f>E83</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="16">
         <f>F83</f>
         <v>1.98</v>
       </c>
-      <c r="G34" s="28">
+      <c r="G34" s="27">
         <f>G83</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="39"/>
-      <c r="G35" s="28"/>
+      <c r="B35" s="62"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="39"/>
-      <c r="G36" s="28"/>
+      <c r="B36" s="62"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="40"/>
-      <c r="C37" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="31">
+      <c r="B37" s="63"/>
+      <c r="C37" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="30">
         <f>SUM(E25:E36)</f>
         <v>2.8528599999999997</v>
       </c>
-      <c r="F37" s="31">
+      <c r="F37" s="30">
         <f>SUM(F25:F36)</f>
         <v>9.0220000000000002</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="31">
         <f>SUM(G25:G36)</f>
         <v>11.067</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
+      <c r="B39" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="21"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="39"/>
+      <c r="B40" s="62"/>
       <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="E40" s="17">
+        <v>130</v>
+      </c>
+      <c r="E40" s="16">
         <v>0.6</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="16">
         <v>0.6</v>
       </c>
-      <c r="G40" s="28">
+      <c r="G40" s="27">
         <v>0.87</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="39"/>
+      <c r="B41" s="62"/>
       <c r="C41" t="s">
-        <v>138</v>
-      </c>
-      <c r="E41" s="17">
+        <v>131</v>
+      </c>
+      <c r="E41" s="16">
         <f>6*7</f>
         <v>42</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="16">
         <f>6*7</f>
         <v>42</v>
       </c>
-      <c r="G41" s="28">
+      <c r="G41" s="27">
         <f>9*7</f>
         <v>63</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="39"/>
+      <c r="B42" s="62"/>
       <c r="C42" t="s">
-        <v>139</v>
-      </c>
-      <c r="E42" s="17">
+        <v>132</v>
+      </c>
+      <c r="E42" s="16">
         <f>0.01*4</f>
         <v>0.04</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="16">
         <f>0.05*4</f>
         <v>0.2</v>
       </c>
-      <c r="G42" s="28">
+      <c r="G42" s="27">
         <f>0.075*4</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="39"/>
+      <c r="B43" s="62"/>
       <c r="C43" t="s">
-        <v>140</v>
-      </c>
-      <c r="E43" s="17">
+        <v>133</v>
+      </c>
+      <c r="E43" s="16">
         <v>1</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F43" s="16">
         <v>1</v>
       </c>
-      <c r="G43" s="28">
+      <c r="G43" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="39"/>
+      <c r="B44" s="62"/>
       <c r="C44" t="s">
-        <v>141</v>
-      </c>
-      <c r="G44" s="28"/>
+        <v>134</v>
+      </c>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="39"/>
+      <c r="B45" s="62"/>
       <c r="C45" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E45" s="17">
+        <v>146</v>
+      </c>
+      <c r="E45" s="16">
         <v>2</v>
       </c>
-      <c r="F45" s="17">
+      <c r="F45" s="16">
         <v>2</v>
       </c>
-      <c r="G45" s="28">
+      <c r="G45" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="39"/>
+      <c r="B46" s="62"/>
       <c r="C46" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E46" s="36">
+        <v>151</v>
+      </c>
+      <c r="E46" s="35">
         <v>1</v>
       </c>
-      <c r="F46" s="36">
+      <c r="F46" s="35">
         <v>1</v>
       </c>
-      <c r="G46" s="34">
+      <c r="G46" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="39"/>
-      <c r="G47" s="28"/>
+      <c r="B47" s="62"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="39"/>
-      <c r="C48" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="39"/>
+      <c r="B49" s="62"/>
       <c r="C49" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="G49" s="28"/>
+        <v>129</v>
+      </c>
+      <c r="G49" s="27"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="39"/>
+      <c r="B50" s="62"/>
       <c r="C50" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G50" s="28"/>
+        <v>154</v>
+      </c>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="39"/>
-      <c r="G51" s="28"/>
+      <c r="B51" s="62"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="40"/>
-      <c r="C52" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="25"/>
-      <c r="E52" s="31">
+      <c r="B52" s="63"/>
+      <c r="C52" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D52" s="24"/>
+      <c r="E52" s="30">
         <f>SUM(E40:E51)</f>
         <v>46.64</v>
       </c>
-      <c r="F52" s="31">
+      <c r="F52" s="30">
         <f>SUM(F40:F51)</f>
         <v>46.800000000000004</v>
       </c>
-      <c r="G52" s="32">
+      <c r="G52" s="31">
         <f>SUM(G40:G51)</f>
         <v>70.17</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="27"/>
+      <c r="B54" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="26"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="39"/>
+      <c r="B55" s="62"/>
       <c r="C55" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="17">
+        <v>132</v>
+      </c>
+      <c r="E55" s="16">
         <f>4*0.001</f>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F55" s="17">
+      <c r="F55" s="16">
         <f>4*0.075</f>
         <v>0.3</v>
       </c>
-      <c r="G55" s="28">
+      <c r="G55" s="27">
         <f>F55</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="39"/>
+      <c r="B56" s="62"/>
       <c r="C56" t="s">
-        <v>140</v>
-      </c>
-      <c r="E56" s="17">
+        <v>133</v>
+      </c>
+      <c r="E56" s="16">
         <v>0.5</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F56" s="16">
         <v>0.5</v>
       </c>
-      <c r="G56" s="28">
+      <c r="G56" s="27">
         <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="39"/>
+      <c r="B57" s="62"/>
       <c r="C57" t="s">
+        <v>134</v>
+      </c>
+      <c r="G57" s="27"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="62"/>
+      <c r="C58" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="16">
+        <v>2</v>
+      </c>
+      <c r="F58" s="16">
+        <v>2</v>
+      </c>
+      <c r="G58" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="62"/>
+      <c r="G59" s="27"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="62"/>
+      <c r="G60" s="27"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="62"/>
+      <c r="C61" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="29"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="62"/>
+      <c r="C62" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="G57" s="28"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="39"/>
-      <c r="C58" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E58" s="17">
+      <c r="E62" s="32">
+        <v>1</v>
+      </c>
+      <c r="F62" s="32">
         <v>2</v>
       </c>
-      <c r="F58" s="17">
+      <c r="G62" s="33">
         <v>2</v>
       </c>
-      <c r="G58" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="39"/>
-      <c r="G59" s="28"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="39"/>
-      <c r="G60" s="28"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="39"/>
-      <c r="C61" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="30"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="39"/>
-      <c r="C62" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E62" s="33">
-        <v>1</v>
-      </c>
-      <c r="F62" s="33">
-        <v>2</v>
-      </c>
-      <c r="G62" s="34">
-        <v>2</v>
-      </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="39"/>
-      <c r="G63" s="28"/>
+      <c r="B63" s="62"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="39"/>
-      <c r="G64" s="28"/>
+      <c r="B64" s="62"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="40"/>
-      <c r="C65" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D65" s="25"/>
-      <c r="E65" s="31">
+      <c r="B65" s="63"/>
+      <c r="C65" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" s="24"/>
+      <c r="E65" s="30">
         <f>SUM(E55:E64)</f>
         <v>3.504</v>
       </c>
-      <c r="F65" s="31">
+      <c r="F65" s="30">
         <f>SUM(F55:F64)</f>
         <v>4.8</v>
       </c>
-      <c r="G65" s="32">
+      <c r="G65" s="31">
         <f>SUM(G55:G64)</f>
         <v>5.8</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D67" s="22"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="27"/>
+      <c r="B67" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="39"/>
+      <c r="B68" s="62"/>
       <c r="C68" t="s">
-        <v>143</v>
-      </c>
-      <c r="E68" s="17">
+        <v>136</v>
+      </c>
+      <c r="E68" s="16">
         <f>3*0.00004</f>
         <v>1.2000000000000002E-4</v>
       </c>
-      <c r="F68" s="17">
+      <c r="F68" s="16">
         <f>3*0.22</f>
         <v>0.66</v>
       </c>
-      <c r="G68" s="28">
+      <c r="G68" s="27">
         <f>3*0.29</f>
         <v>0.86999999999999988</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B69" s="39"/>
+      <c r="B69" s="62"/>
       <c r="C69" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E69" s="17">
+        <v>148</v>
+      </c>
+      <c r="E69" s="16">
         <v>2</v>
       </c>
-      <c r="F69" s="17">
+      <c r="F69" s="16">
         <v>2</v>
       </c>
-      <c r="G69" s="28">
+      <c r="G69" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B70" s="39"/>
-      <c r="G70" s="28"/>
+      <c r="B70" s="62"/>
+      <c r="G70" s="27"/>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B71" s="39"/>
-      <c r="G71" s="28"/>
+      <c r="B71" s="62"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" s="39"/>
-      <c r="G72" s="28"/>
+      <c r="B72" s="62"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B73" s="39"/>
-      <c r="C73" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D73" s="23"/>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-      <c r="G73" s="30"/>
+      <c r="B73" s="62"/>
+      <c r="C73" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D73" s="22"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="29"/>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B74" s="39"/>
-      <c r="G74" s="28"/>
+      <c r="B74" s="62"/>
+      <c r="G74" s="27"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B75" s="39"/>
-      <c r="G75" s="28"/>
+      <c r="B75" s="62"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B76" s="39"/>
-      <c r="G76" s="28"/>
+      <c r="B76" s="62"/>
+      <c r="G76" s="27"/>
     </row>
     <row r="77" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="40"/>
-      <c r="C77" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D77" s="25"/>
-      <c r="E77" s="31">
+      <c r="B77" s="63"/>
+      <c r="C77" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D77" s="24"/>
+      <c r="E77" s="30">
         <f>SUM(E68:E76)</f>
         <v>2.0001199999999999</v>
       </c>
-      <c r="F77" s="31">
+      <c r="F77" s="30">
         <f>SUM(F68:F76)</f>
         <v>2.66</v>
       </c>
-      <c r="G77" s="32">
+      <c r="G77" s="31">
         <f>SUM(G68:G76)</f>
         <v>3.87</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="79" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B79" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D79" s="22"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="26"/>
-      <c r="G79" s="27"/>
+      <c r="B79" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D79" s="21"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="26"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B80" s="39"/>
+      <c r="B80" s="62"/>
       <c r="C80" t="s">
-        <v>144</v>
-      </c>
-      <c r="E80" s="17">
+        <v>137</v>
+      </c>
+      <c r="E80" s="16">
         <f>3*0.0015</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="F80" s="17">
+      <c r="F80" s="16">
         <f>3*0.66</f>
         <v>1.98</v>
       </c>
-      <c r="G80" s="28">
+      <c r="G80" s="27">
         <f>3*0.9</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B81" s="39"/>
+      <c r="B81" s="62"/>
       <c r="C81" s="9"/>
       <c r="E81"/>
       <c r="F81"/>
-      <c r="G81" s="37"/>
+      <c r="G81" s="36"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B82" s="39"/>
+      <c r="B82" s="62"/>
       <c r="C82" s="9"/>
       <c r="E82"/>
       <c r="F82"/>
-      <c r="G82" s="37"/>
+      <c r="G82" s="36"/>
     </row>
     <row r="83" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="40"/>
-      <c r="C83" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D83" s="25"/>
-      <c r="E83" s="31">
+      <c r="B83" s="63"/>
+      <c r="C83" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D83" s="24"/>
+      <c r="E83" s="30">
         <f>SUM(E80:E82)</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="F83" s="31">
+      <c r="F83" s="30">
         <f>SUM(F80:F82)</f>
         <v>1.98</v>
       </c>
-      <c r="G83" s="32">
+      <c r="G83" s="31">
         <f>SUM(G80:G82)</f>
         <v>2.7</v>
       </c>
@@ -4052,7 +4203,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4237,25 +4388,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="60">
         <v>470</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="57" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="58">
         <v>10</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="59" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4307,7 +4459,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -4323,23 +4475,23 @@
       <c r="A30" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="56">
         <f>B15+B13+B29/1000*B22</f>
         <v>18.879709716755894</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="57" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="58">
         <f>B16-B13-B29/1000*B22</f>
         <v>-15.579709716755893</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="59" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4357,10 +4509,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77871942-014F-4601-9E14-5BC8E39F3C94}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4518,6 +4670,9 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
+      <c r="D8" t="s">
+        <v>231</v>
+      </c>
       <c r="L8">
         <v>4</v>
       </c>
@@ -4693,7 +4848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -4705,7 +4860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -4717,7 +4872,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -4729,12 +4884,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -4745,7 +4900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -4755,10 +4910,13 @@
       <c r="C24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>232</v>
       </c>
       <c r="B25" s="4">
         <f>(B24-1.76)/6.02</f>
@@ -4768,7 +4926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -4780,12 +4938,79 @@
         <v>21</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>86.9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>232</v>
+      </c>
+      <c r="B31" s="4">
+        <f>(B30-1.76)/6.02</f>
+        <v>14.142857142857144</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="3">
+        <f>B29/2^B31*1000</f>
+        <v>0.27640492683835022</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B37" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B38" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4797,10 +5022,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F83BAB-D15A-47C8-9B74-5014433A0DBB}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4809,704 +5034,486 @@
     <col min="2" max="2" width="43.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <f>C3/2^C4</f>
+        <v>1.220703125E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D7" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E7" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F7" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G7" s="19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="D5" s="3">
-        <f>(1-C5)*E5</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <f>(1+C5)*E5</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="39">
+        <v>1E-3</v>
+      </c>
+      <c r="D8" s="15">
+        <f>(1-C8)*E8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0</v>
+      </c>
+      <c r="F8" s="15">
+        <f>(1+C8)*E8</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="55">
+        <f>E8*E9/(E8+E9)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="65"/>
       <c r="B9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="6">
-        <f>F5-D5</f>
-        <v>0.19999999999999929</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C9" s="40">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="37">
+        <f>(1-C9)*E9</f>
+        <v>4985.01</v>
+      </c>
+      <c r="E9" s="37">
+        <v>4990</v>
+      </c>
+      <c r="F9" s="37">
+        <f>(1+C9)*E9</f>
+        <v>4994.99</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="65"/>
       <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="16">
+        <v>40</v>
+      </c>
+      <c r="E10" s="16">
         <v>100</v>
       </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11">
-        <f>C9/E5*2^C10</f>
-        <v>163.83999999999941</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="F10" s="16">
+        <v>125</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="66"/>
+      <c r="B11" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="18">
+        <f>1+(D8+D10)/F9</f>
+        <v>1.0080080240400882</v>
+      </c>
+      <c r="E11" s="18">
+        <f>1+(E8+E10)/E9</f>
+        <v>1.0200400801603207</v>
+      </c>
+      <c r="F11" s="18">
+        <f>1+(F8+F10)/D9</f>
+        <v>1.0250751753757765</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="4">
-        <f>LOG(C11,2)</f>
-        <v>7.3561438102252703</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="39">
+        <v>1E-3</v>
+      </c>
+      <c r="D12" s="38">
+        <f>(1-C12)*E12</f>
+        <v>45254.7</v>
+      </c>
+      <c r="E12" s="38">
+        <v>45300</v>
+      </c>
+      <c r="F12" s="38">
+        <f>(1+C12)*E12</f>
+        <v>45345.299999999996</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="55">
+        <f>E12*E13/(E12+E13)</f>
+        <v>4494.8697554185719</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="68"/>
       <c r="B13" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="4">
-        <f>C10-C12</f>
-        <v>4.6438561897747297</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C13" s="40">
+        <v>1E-3</v>
+      </c>
+      <c r="D13" s="37">
+        <f>(1-C13)*E13</f>
+        <v>4985.01</v>
+      </c>
+      <c r="E13" s="37">
+        <f>E9</f>
+        <v>4990</v>
+      </c>
+      <c r="F13" s="37">
+        <f>(1+C13)*E13</f>
+        <v>4994.99</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="68"/>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="16">
+        <v>40</v>
+      </c>
+      <c r="E14" s="16">
+        <v>100</v>
+      </c>
+      <c r="F14" s="16">
+        <v>125</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="69"/>
+      <c r="B15" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="18">
+        <f>1+(D12+D14)/F13</f>
+        <v>10.068026162214538</v>
+      </c>
+      <c r="E15" s="18">
+        <f>1+(E12+E14)/E13</f>
+        <v>10.098196392785571</v>
+      </c>
+      <c r="F15" s="18">
+        <f>1+(F12+F14)/D13</f>
+        <v>10.121405975113388</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="39">
+        <v>1E-3</v>
+      </c>
+      <c r="D16" s="38">
+        <f>(1-C16)*E16</f>
+        <v>242757</v>
+      </c>
+      <c r="E16" s="38">
+        <v>243000</v>
+      </c>
+      <c r="F16" s="38">
+        <f>(1+C16)*E16</f>
+        <v>243242.99999999997</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="55">
+        <f>E16*E17/(E16+E17)</f>
+        <v>4889.5923222710589</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="71"/>
       <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="10">
+        <v>104</v>
+      </c>
+      <c r="C17" s="40">
         <v>1E-3</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="37">
         <f>(1-C17)*E17</f>
-        <v>4.9950000000000001</v>
-      </c>
-      <c r="E17" s="3">
-        <v>5</v>
-      </c>
-      <c r="F17" s="3">
+        <v>4985.01</v>
+      </c>
+      <c r="E17" s="37">
+        <f>E9</f>
+        <v>4990</v>
+      </c>
+      <c r="F17" s="37">
         <f>(1+C17)*E17</f>
-        <v>5.004999999999999</v>
-      </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+        <v>4994.99</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="71"/>
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="16">
+        <v>40</v>
+      </c>
+      <c r="E18" s="16">
+        <v>100</v>
+      </c>
+      <c r="F18" s="16">
+        <v>125</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="72"/>
+      <c r="B19" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="18">
+        <f>1+(D16+D18)/D17</f>
+        <v>49.705418845699405</v>
+      </c>
+      <c r="E19" s="18">
+        <f>1+(E16+E18)/E17</f>
+        <v>49.717434869739478</v>
+      </c>
+      <c r="F19" s="18">
+        <f>1+(F16+F18)/D17</f>
+        <v>49.819962246815948</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="39">
+        <v>1E-3</v>
+      </c>
+      <c r="D20" s="38">
+        <f>(1-C20)*E20</f>
+        <v>498501</v>
+      </c>
+      <c r="E20" s="38">
+        <v>499000</v>
+      </c>
+      <c r="F20" s="38">
+        <f>(1+C20)*E20</f>
+        <v>499498.99999999994</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="55">
+        <f>E20*E21/(E20+E21)</f>
+        <v>4940.5940594059402</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="74"/>
       <c r="B21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="6">
-        <f>F17-D17</f>
-        <v>9.9999999999988987E-3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C21" s="40">
+        <v>1E-3</v>
+      </c>
+      <c r="D21" s="37">
+        <f>(1-C21)*E21</f>
+        <v>4985.01</v>
+      </c>
+      <c r="E21" s="37">
+        <f>E9</f>
+        <v>4990</v>
+      </c>
+      <c r="F21" s="37">
+        <f>(1+C21)*E21</f>
+        <v>4994.99</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="74"/>
       <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="16">
+        <v>40</v>
+      </c>
+      <c r="E22" s="16">
         <v>100</v>
       </c>
-      <c r="C22">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23">
-        <f>C21/E17*2^C22</f>
-        <v>8.1919999999990978</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="4">
-        <f>LOG(C23,2)</f>
-        <v>3.034215715337754</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="4">
-        <f>C22-C24</f>
-        <v>8.9657842846622451</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="F22" s="16">
+        <v>125</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="75"/>
+      <c r="B23" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30">
-        <f>C28/2^C29</f>
-        <v>1.220703125E-3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="43">
-        <v>1E-3</v>
-      </c>
-      <c r="D33" s="16">
-        <f>(1-C33)*E33</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="16">
-        <v>0</v>
-      </c>
-      <c r="F33" s="16">
-        <f>(1+C33)*E33</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" s="74">
-        <f>E33*E34/(E33+E34)</f>
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
-      <c r="B34" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="44">
-        <v>1E-3</v>
-      </c>
-      <c r="D34" s="41">
-        <f>(1-C34)*E34</f>
-        <v>4985.01</v>
-      </c>
-      <c r="E34" s="41">
-        <v>4990</v>
-      </c>
-      <c r="F34" s="41">
-        <f>(1+C34)*E34</f>
-        <v>4994.99</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="17">
-        <v>40</v>
-      </c>
-      <c r="E35" s="17">
-        <v>100</v>
-      </c>
-      <c r="F35" s="17">
-        <v>125</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="47"/>
-      <c r="B36" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="19">
-        <f>1+(D33+D35)/F34</f>
-        <v>1.0080080240400882</v>
-      </c>
-      <c r="E36" s="19">
-        <f>1+(E33+E35)/E34</f>
-        <v>1.0200400801603207</v>
-      </c>
-      <c r="F36" s="19">
-        <f>1+(F33+F35)/D34</f>
-        <v>1.0250751753757765</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="43">
-        <v>1E-3</v>
-      </c>
-      <c r="D37" s="42">
-        <f>(1-C37)*E37</f>
-        <v>45254.7</v>
-      </c>
-      <c r="E37" s="42">
-        <v>45300</v>
-      </c>
-      <c r="F37" s="42">
-        <f>(1+C37)*E37</f>
-        <v>45345.299999999996</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I37" s="74">
-        <f>E37*E38/(E37+E38)</f>
-        <v>4494.8697554185719</v>
-      </c>
-      <c r="J37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="49"/>
-      <c r="B38" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="44">
-        <v>1E-3</v>
-      </c>
-      <c r="D38" s="41">
-        <f>(1-C38)*E38</f>
-        <v>4985.01</v>
-      </c>
-      <c r="E38" s="41">
-        <f>E34</f>
-        <v>4990</v>
-      </c>
-      <c r="F38" s="41">
-        <f>(1+C38)*E38</f>
-        <v>4994.99</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="49"/>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="17">
-        <v>40</v>
-      </c>
-      <c r="E39" s="17">
-        <v>100</v>
-      </c>
-      <c r="F39" s="17">
-        <v>125</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="50"/>
-      <c r="B40" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="19">
-        <f>1+(D37+D39)/F38</f>
-        <v>10.068026162214538</v>
-      </c>
-      <c r="E40" s="19">
-        <f>1+(E37+E39)/E38</f>
-        <v>10.098196392785571</v>
-      </c>
-      <c r="F40" s="19">
-        <f>1+(F37+F39)/D38</f>
-        <v>10.121405975113388</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" s="43">
-        <v>1E-3</v>
-      </c>
-      <c r="D41" s="42">
-        <f>(1-C41)*E41</f>
-        <v>242757</v>
-      </c>
-      <c r="E41" s="42">
-        <v>243000</v>
-      </c>
-      <c r="F41" s="42">
-        <f>(1+C41)*E41</f>
-        <v>243242.99999999997</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="74">
-        <f>E41*E42/(E41+E42)</f>
-        <v>4889.5923222710589</v>
-      </c>
-      <c r="J41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="52"/>
-      <c r="B42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="44">
-        <v>1E-3</v>
-      </c>
-      <c r="D42" s="41">
-        <f>(1-C42)*E42</f>
-        <v>4985.01</v>
-      </c>
-      <c r="E42" s="41">
-        <f>E34</f>
-        <v>4990</v>
-      </c>
-      <c r="F42" s="41">
-        <f>(1+C42)*E42</f>
-        <v>4994.99</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="52"/>
-      <c r="B43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="17">
-        <v>40</v>
-      </c>
-      <c r="E43" s="17">
-        <v>100</v>
-      </c>
-      <c r="F43" s="17">
-        <v>125</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="53"/>
-      <c r="B44" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="19">
-        <f>1+(D41+D43)/D42</f>
-        <v>49.705418845699405</v>
-      </c>
-      <c r="E44" s="19">
-        <f>1+(E41+E43)/E42</f>
-        <v>49.717434869739478</v>
-      </c>
-      <c r="F44" s="19">
-        <f>1+(F41+F43)/D42</f>
-        <v>49.819962246815948</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" s="43">
-        <v>1E-3</v>
-      </c>
-      <c r="D45" s="42">
-        <f>(1-C45)*E45</f>
-        <v>498501</v>
-      </c>
-      <c r="E45" s="42">
-        <v>499000</v>
-      </c>
-      <c r="F45" s="42">
-        <f>(1+C45)*E45</f>
-        <v>499498.99999999994</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I45" s="74">
-        <f>E45*E46/(E45+E46)</f>
-        <v>4940.5940594059402</v>
-      </c>
-      <c r="J45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="55"/>
-      <c r="B46" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="44">
-        <v>1E-3</v>
-      </c>
-      <c r="D46" s="41">
-        <f>(1-C46)*E46</f>
-        <v>4985.01</v>
-      </c>
-      <c r="E46" s="41">
-        <f>E34</f>
-        <v>4990</v>
-      </c>
-      <c r="F46" s="41">
-        <f>(1+C46)*E46</f>
-        <v>4994.99</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="55"/>
-      <c r="B47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="17">
-        <v>40</v>
-      </c>
-      <c r="E47" s="17">
-        <v>100</v>
-      </c>
-      <c r="F47" s="17">
-        <v>125</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="56"/>
-      <c r="B48" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="19">
-        <f>1+(D45+D47)/F46</f>
+      <c r="D23" s="18">
+        <f>1+(D20+D22)/F21</f>
         <v>100.80820782423989</v>
       </c>
-      <c r="E48" s="19">
-        <f>1+(E45+E47)/E46</f>
+      <c r="E23" s="18">
+        <f>1+(E20+E22)/E21</f>
         <v>101.02004008016031</v>
       </c>
-      <c r="F48" s="19">
-        <f>1+(F45+F47)/D46</f>
+      <c r="F23" s="18">
+        <f>1+(F20+F22)/D21</f>
         <v>101.22527537557596</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5515,7 +5522,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5530,7 +5537,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -5561,35 +5568,35 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B5">
         <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G5">
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -5598,10 +5605,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" t="s">
         <v>183</v>
-      </c>
-      <c r="F6" t="s">
-        <v>190</v>
       </c>
       <c r="G6">
         <v>-15</v>
@@ -5612,7 +5619,7 @@
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B7">
         <v>1.2130000000000001</v>
@@ -5621,10 +5628,10 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <v>1.2130000000000001</v>
@@ -5635,44 +5642,44 @@
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="49">
+        <v>47.5</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="66">
+      <c r="G8" s="49">
         <v>47.5</v>
       </c>
-      <c r="C8" s="67" t="s">
-        <v>171</v>
-      </c>
-      <c r="F8" t="s">
-        <v>192</v>
-      </c>
-      <c r="G8" s="66">
-        <v>47.5</v>
-      </c>
-      <c r="H8" s="67" t="s">
-        <v>171</v>
+      <c r="H8" s="50" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B9">
         <f>B8*(B6/B7-1)</f>
         <v>539.88664468260504</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F9" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G9">
         <f>-1*G8*G6/G7</f>
         <v>587.38664468260504</v>
       </c>
       <c r="H9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -5680,25 +5687,25 @@
       <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="66">
+      <c r="B11" s="49">
         <v>536</v>
       </c>
-      <c r="C11" s="67" t="s">
-        <v>171</v>
+      <c r="C11" s="50" t="s">
+        <v>164</v>
       </c>
       <c r="F11" t="s">
-        <v>194</v>
-      </c>
-      <c r="G11" s="66">
+        <v>187</v>
+      </c>
+      <c r="G11" s="49">
         <v>576</v>
       </c>
-      <c r="H11" s="67" t="s">
-        <v>171</v>
+      <c r="H11" s="50" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B12">
         <f>(1+B11/B8)*B7</f>
@@ -5708,7 +5715,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G12">
         <f>-G11/G8*G7</f>
@@ -5720,15 +5727,15 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -5737,7 +5744,7 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G16">
         <v>5</v>
@@ -5748,88 +5755,88 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B17">
         <v>0.08</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F17" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="G17">
         <v>0.01</v>
       </c>
       <c r="H17" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I17" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B18">
         <f>B6/(B16*0.64)*B17</f>
         <v>0.375</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F18" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G18">
         <f>(G16-G6)/(G16*0.64)*G17</f>
         <v>6.25E-2</v>
       </c>
       <c r="H18" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B19">
         <f>0.2*B18</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F19" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G19">
         <f>0.2*G18</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="H19" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>205</v>
-      </c>
-      <c r="B20" s="68">
+        <v>198</v>
+      </c>
+      <c r="B20">
         <v>1.25</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>205</v>
-      </c>
-      <c r="G20" s="68">
+        <v>198</v>
+      </c>
+      <c r="G20">
         <v>1.25</v>
       </c>
       <c r="H20" t="s">
@@ -5838,43 +5845,43 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>206</v>
-      </c>
-      <c r="B21" s="69">
+        <v>199</v>
+      </c>
+      <c r="B21" s="51">
         <f>B16*(B6-B16)/(B19*B20*B6)</f>
         <v>35.55555555555555</v>
       </c>
-      <c r="C21" s="70" t="s">
-        <v>207</v>
+      <c r="C21" s="52" t="s">
+        <v>200</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F21" t="s">
-        <v>208</v>
-      </c>
-      <c r="G21" s="70">
+        <v>201</v>
+      </c>
+      <c r="G21" s="52">
         <f>G16*G6/(G19*G20*(G6-G16))</f>
         <v>240</v>
       </c>
-      <c r="H21" s="70" t="s">
-        <v>207</v>
+      <c r="H21" s="52" t="s">
+        <v>200</v>
       </c>
       <c r="I21" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B25">
         <v>5.0000000000000001E-3</v>
@@ -5883,7 +5890,7 @@
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="G25">
         <v>5.0000000000000001E-3</v>
@@ -5894,29 +5901,29 @@
     </row>
     <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>212</v>
-      </c>
-      <c r="B26" s="71">
+        <v>205</v>
+      </c>
+      <c r="B26" s="53">
         <f>B17*(B6-B16)/(B20*B25*B6)</f>
         <v>8.5333333333333332</v>
       </c>
-      <c r="C26" s="67" t="s">
-        <v>211</v>
+      <c r="C26" s="50" t="s">
+        <v>204</v>
       </c>
       <c r="F26" t="s">
-        <v>213</v>
-      </c>
-      <c r="G26" s="66">
+        <v>206</v>
+      </c>
+      <c r="G26" s="49">
         <f>G17*G6/(G20*G25*(G6-G16))</f>
         <v>1.2</v>
       </c>
-      <c r="H26" s="67" t="s">
-        <v>211</v>
+      <c r="H26" s="50" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B27">
         <v>0.01</v>
@@ -5925,7 +5932,7 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G27">
         <v>0.01</v>
@@ -5936,7 +5943,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B28">
         <f>B17*B27</f>
@@ -5946,7 +5953,7 @@
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G28">
         <f>G17*G27</f>
@@ -5958,52 +5965,52 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>220</v>
-      </c>
-      <c r="B32" s="72">
+        <v>213</v>
+      </c>
+      <c r="B32" s="54">
         <f>0.0000068/(B11*1000)</f>
         <v>1.2686567164179104E-11</v>
       </c>
-      <c r="C32" s="73" t="s">
-        <v>221</v>
+      <c r="C32" t="s">
+        <v>214</v>
       </c>
       <c r="F32" t="s">
-        <v>224</v>
-      </c>
-      <c r="G32" s="72">
+        <v>217</v>
+      </c>
+      <c r="G32" s="54">
         <f>0.0000075/(G11*1000)</f>
         <v>1.3020833333333334E-11</v>
       </c>
-      <c r="H32" s="73" t="s">
-        <v>221</v>
+      <c r="H32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B33">
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F33" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G33">
         <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -6018,7 +6025,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6030,7 +6037,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6047,7 +6054,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>3</v>
@@ -6058,20 +6065,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <f>3*0.00004</f>
         <v>1.2000000000000002E-4</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <f>3*0.22</f>
         <v>0.66</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="16">
         <f>3*0.29</f>
         <v>0.86999999999999988</v>
       </c>
@@ -6081,43 +6088,43 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <f>C4+C5</f>
         <v>1.0001199999999999</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <f>D4+D5</f>
         <v>1.6600000000000001</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>E4+E5</f>
         <v>1.8699999999999999</v>
       </c>
@@ -6126,47 +6133,47 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>11.9</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>12</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>12.1</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>4.9950000000000001</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>5</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>5.0049999999999999</v>
       </c>
       <c r="F9" t="s">
@@ -6174,23 +6181,23 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="17">
+        <v>162</v>
+      </c>
+      <c r="C11" s="16">
         <f>C8-E9</f>
         <v>6.8950000000000005</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <f>D8-D9</f>
         <v>7</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <f>E8-C9</f>
         <v>7.1049999999999995</v>
       </c>
@@ -6200,89 +6207,89 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="58">
+        <v>171</v>
+      </c>
+      <c r="C12" s="41">
         <f>C11/E6</f>
         <v>3.6871657754010698</v>
       </c>
-      <c r="D12" s="59">
+      <c r="D12" s="42">
         <f>D11/D6</f>
         <v>4.2168674698795181</v>
       </c>
-      <c r="E12" s="60">
+      <c r="E12" s="43">
         <f>E11/C6</f>
         <v>7.1041475022997247</v>
       </c>
       <c r="F12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="61">
+      <c r="C14" s="16"/>
+      <c r="D14" s="44">
         <f>(D8-D9)/(D6)</f>
         <v>4.2168674698795181</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="16"/>
       <c r="F14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="62" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="63">
+      <c r="A16" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="46">
         <v>0.01</v>
       </c>
-      <c r="C16" s="64">
+      <c r="C16" s="47">
         <f>(1-B16)*D16</f>
         <v>4.1777999999999995</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="47">
         <v>4.22</v>
       </c>
-      <c r="E16" s="64">
+      <c r="E16" s="47">
         <f>(1+B16)*D16</f>
         <v>4.2622</v>
       </c>
-      <c r="F16" s="65" t="s">
-        <v>171</v>
+      <c r="F16" s="48" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C17" s="35">
+        <v>169</v>
+      </c>
+      <c r="C17" s="34">
         <f>C11/E16-E4</f>
         <v>0.74770916428135736</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="34">
         <f>D11/D16-D4</f>
         <v>0.99876777251184834</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="34">
         <f>E11/C16-C4</f>
         <v>1.700535847575279</v>
       </c>
@@ -6290,7 +6297,7 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -6334,12 +6341,12 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -6348,12 +6355,12 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -6362,12 +6369,12 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -6378,7 +6385,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -6431,7 +6438,7 @@
         <v>3225806.4516129033</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add series termination to nCS and mux select. doing checklists
</commit_message>
<xml_diff>
--- a/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
+++ b/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\0 Documentation\1 Design Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F2F73B-A639-4E87-909B-FC53C3A731D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F24DC3-16FA-4475-BADA-C447BA7B1D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="3" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
   </bookViews>
@@ -2758,9 +2758,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>517943</xdr:colOff>
+      <xdr:colOff>514133</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>71165</xdr:rowOff>
+      <xdr:rowOff>59735</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5025,7 +5025,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5521,8 +5521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A480CAEC-DF0D-4E76-B5A5-4113DE0E6389}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
continuing testing, committing changes
</commit_message>
<xml_diff>
--- a/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
+++ b/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\0 Documentation\1 Design Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A34942A-FC4E-47C2-A8EA-A294DF062B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476390F-6CED-4F67-9A6E-5E394553EE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="7" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="8" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="6" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="285">
   <si>
     <t>Digital Input Protection</t>
   </si>
@@ -888,9 +888,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -901,6 +898,51 @@
   </si>
   <si>
     <t>+/- 15V boost quiescent current</t>
+  </si>
+  <si>
+    <t>Review Checklist</t>
+  </si>
+  <si>
+    <t>Tense -- past vs present</t>
+  </si>
+  <si>
+    <t>Rubric</t>
+  </si>
+  <si>
+    <t>Capitalization on figures and tables captions</t>
+  </si>
+  <si>
+    <t>Abbreviations first instance</t>
+  </si>
+  <si>
+    <t>Requirements -- bolded shalls</t>
+  </si>
+  <si>
+    <t>Figures -- text readable</t>
+  </si>
+  <si>
+    <t>SI unitx used everywhere</t>
+  </si>
+  <si>
+    <t>No more todos left</t>
+  </si>
+  <si>
+    <t>No watermark</t>
+  </si>
+  <si>
+    <t>All abbreviations are in the list</t>
+  </si>
+  <si>
+    <t>All tables are referenced in the text</t>
+  </si>
+  <si>
+    <t>All figures are referenced in the text</t>
+  </si>
+  <si>
+    <t>Sections make sense, no further division needed</t>
+  </si>
+  <si>
+    <t>All sections in rubric are present in report</t>
   </si>
 </sst>
 </file>
@@ -1451,7 +1493,37 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3585,7 +3657,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="67"/>
       <c r="C11" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E11" s="16">
         <f>(E43+E53)*15/_RAIL_5V/EFF_12V_BOOST</f>
@@ -3885,7 +3957,7 @@
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="67"/>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E36" s="16">
         <v>5</v>
@@ -4007,7 +4079,7 @@
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="67"/>
       <c r="C47" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E47" s="16">
         <v>2.5</v>
@@ -4259,7 +4331,7 @@
     <mergeCell ref="B58:B63"/>
   </mergeCells>
   <conditionalFormatting sqref="E15:G15">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>499.99</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6992,7 +7064,7 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -7263,15 +7335,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4773A798-633B-4D8D-9FC8-9ECE55BCD182}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
@@ -7361,7 +7433,7 @@
         <v>257</v>
       </c>
       <c r="B11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7380,7 +7452,7 @@
         <v>265</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -7404,18 +7476,138 @@
         <v>262</v>
       </c>
       <c r="B16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" t="s">
         <v>266</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>274</v>
+      </c>
+      <c r="B22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>276</v>
+      </c>
+      <c r="B24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>277</v>
+      </c>
+      <c r="B25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>278</v>
+      </c>
+      <c r="B26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>279</v>
+      </c>
+      <c r="B27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>280</v>
+      </c>
+      <c r="B28" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>282</v>
+      </c>
+      <c r="B29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>281</v>
+      </c>
+      <c r="B30" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>284</v>
+      </c>
+      <c r="B32" t="s">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B16">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="In Progress">
+  <conditionalFormatting sqref="B2:B160">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
copy eval board to daq device schematics. updated power budget. continued design for daq device
</commit_message>
<xml_diff>
--- a/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
+++ b/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\0 Documentation\1 Design Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476390F-6CED-4F67-9A6E-5E394553EE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCEFB1E-66AD-4605-BF80-8D5390567D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="8" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="3" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="6" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="320">
   <si>
     <t>Digital Input Protection</t>
   </si>
@@ -474,9 +474,6 @@
     <t>INA821 In-amp</t>
   </si>
   <si>
-    <t>RC4580 Op-amp x 7</t>
-  </si>
-  <si>
     <t>DG408 8:1 mux x 4</t>
   </si>
   <si>
@@ -489,15 +486,9 @@
     <t>MCP33151-10 ADC x 3 (AVDD)</t>
   </si>
   <si>
-    <t>MCP23008 IO Expansion x 3</t>
-  </si>
-  <si>
     <t>Relay driver HIGH pull-down in driver</t>
   </si>
   <si>
-    <t>-12V inverting converter quiescent draw</t>
-  </si>
-  <si>
     <t>+3V3 (LDO on Teensy)</t>
   </si>
   <si>
@@ -522,18 +513,12 @@
     <t>Power Budget</t>
   </si>
   <si>
-    <t>+12V LDO quiescent draw</t>
-  </si>
-  <si>
     <t>+1V8_A LDO quiescent draw</t>
   </si>
   <si>
     <t>Must stay below 500mA to respect USB 2.0 spec!</t>
   </si>
   <si>
-    <t>+5V_A (precision shunt reference)</t>
-  </si>
-  <si>
     <t>Teensy 4.1 consumption</t>
   </si>
   <si>
@@ -888,27 +873,18 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>removed :)</t>
   </si>
   <si>
     <t>DG409 dual 4:1 mux x 5</t>
   </si>
   <si>
-    <t>+/- 15V boost quiescent current</t>
-  </si>
-  <si>
     <t>Review Checklist</t>
   </si>
   <si>
     <t>Tense -- past vs present</t>
   </si>
   <si>
-    <t>Rubric</t>
-  </si>
-  <si>
     <t>Capitalization on figures and tables captions</t>
   </si>
   <si>
@@ -943,6 +919,135 @@
   </si>
   <si>
     <t>All sections in rubric are present in report</t>
+  </si>
+  <si>
+    <t>skipping, looked good on two readthroughs</t>
+  </si>
+  <si>
+    <t>update main block diagram resolution</t>
+  </si>
+  <si>
+    <t>Rubric Sections</t>
+  </si>
+  <si>
+    <t>Present?</t>
+  </si>
+  <si>
+    <t>Title page</t>
+  </si>
+  <si>
+    <t>Acknowledgements</t>
+  </si>
+  <si>
+    <t>Table of Contents</t>
+  </si>
+  <si>
+    <t>List of abbreviations</t>
+  </si>
+  <si>
+    <t>Plan for Next Semester</t>
+  </si>
+  <si>
+    <t>use of non-renewable resources</t>
+  </si>
+  <si>
+    <t>environmental benefits</t>
+  </si>
+  <si>
+    <t>safety and risk</t>
+  </si>
+  <si>
+    <t>benefits to society</t>
+  </si>
+  <si>
+    <t>Appendices</t>
+  </si>
+  <si>
+    <t>Check rubric grading elements</t>
+  </si>
+  <si>
+    <t>1 inch margins</t>
+  </si>
+  <si>
+    <t>11pt font</t>
+  </si>
+  <si>
+    <t>Rubric Grading</t>
+  </si>
+  <si>
+    <t>Formatting and presentation</t>
+  </si>
+  <si>
+    <t>Self-graded level</t>
+  </si>
+  <si>
+    <t>exceeds expectations</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Organization and flow</t>
+  </si>
+  <si>
+    <t>clearly meets expectations  / exceeds expectations</t>
+  </si>
+  <si>
+    <t>Technical content (intro, background)</t>
+  </si>
+  <si>
+    <t>Technical content (problem, design, results, testing)</t>
+  </si>
+  <si>
+    <t>clearly meets expectations</t>
+  </si>
+  <si>
+    <t>Plan for next semester</t>
+  </si>
+  <si>
+    <t>Impact on society and environment</t>
+  </si>
+  <si>
+    <t>+/- 15V (TPS65131) boost quiescent current</t>
+  </si>
+  <si>
+    <t>+15V boost --&gt; +12V LDO</t>
+  </si>
+  <si>
+    <t>-15V boost inverting --&gt; -12V LDO</t>
+  </si>
+  <si>
+    <t>+5V_A (precision shunt reference) quiescent bias</t>
+  </si>
+  <si>
+    <t>+5V_A rail load</t>
+  </si>
+  <si>
+    <t>MCP9700T temperature sensor quiescent draw</t>
+  </si>
+  <si>
+    <t>MCP23008 IO Expansion x 4</t>
+  </si>
+  <si>
+    <t>-12V LDO quiescent draw</t>
+  </si>
+  <si>
+    <t>Op Amps</t>
+  </si>
+  <si>
+    <t>RC4580</t>
+  </si>
+  <si>
+    <t>TLV2172</t>
+  </si>
+  <si>
+    <t>Results in too much current!</t>
+  </si>
+  <si>
+    <t>TLV2172 Op-amp x 8</t>
+  </si>
+  <si>
+    <t>+12V LDO quiescent draw (LDK320AM120R)</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1321,12 +1426,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1443,6 +1579,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1493,37 +1647,7 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2653,6 +2777,66 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>384928</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>53850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>18526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695D9FD6-C8D5-58D9-FF84-5B82E5397AC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8287732" y="3182599"/>
+          <a:ext cx="3962399" cy="2370364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2857,7 +3041,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2898,7 +3082,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2958,7 +3142,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3087,7 +3271,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3441,10 +3625,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3461,7 +3645,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3483,7 +3667,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="76" t="s">
         <v>120</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -3493,143 +3677,154 @@
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
       <c r="G4" s="25"/>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="68" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E5" s="16">
-        <v>2</v>
+        <v>1.05</v>
       </c>
       <c r="F5" s="16">
-        <v>2</v>
+        <v>1.06</v>
       </c>
       <c r="G5" s="26">
-        <v>3</v>
-      </c>
-      <c r="K5" t="str">
+        <v>1.07</v>
+      </c>
+      <c r="K5" s="69" t="str">
         <f>B4</f>
         <v>+5V</v>
       </c>
       <c r="L5" s="31">
         <f>E15</f>
-        <v>321.00286</v>
+        <v>263.89880999999997</v>
       </c>
       <c r="M5" s="31">
         <f>F15</f>
-        <v>327.77199999999999</v>
-      </c>
-      <c r="N5" s="31">
+        <v>286.62175000000002</v>
+      </c>
+      <c r="N5" s="70">
         <f>G15</f>
-        <v>446.5795</v>
+        <v>368.49974999999995</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="67"/>
+      <c r="B6" s="77"/>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E6" s="16">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F6" s="16">
         <v>100</v>
       </c>
       <c r="G6" s="26">
-        <v>100</v>
-      </c>
-      <c r="K6" t="str">
+        <v>110</v>
+      </c>
+      <c r="K6" s="69" t="str">
         <f>B17</f>
         <v>+3V3</v>
       </c>
       <c r="L6" s="31">
         <f>E30</f>
-        <v>2.8528599999999997</v>
+        <v>4.1608599999999996</v>
       </c>
       <c r="M6" s="31">
         <f t="shared" ref="M6:N6" si="0">F30</f>
-        <v>9.0220000000000002</v>
-      </c>
-      <c r="N6" s="31">
+        <v>11.328000000000001</v>
+      </c>
+      <c r="N6" s="70">
         <f t="shared" si="0"/>
-        <v>11.067</v>
+        <v>12.381999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="67"/>
-      <c r="G7" s="26"/>
-      <c r="K7" t="str">
+      <c r="B7" s="77"/>
+      <c r="C7" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="K7" s="69" t="str">
         <f>B32</f>
         <v>+12V</v>
       </c>
       <c r="L7" s="31">
-        <f>E43</f>
-        <v>51.64</v>
+        <f>E45</f>
+        <v>35.158119999999997</v>
       </c>
       <c r="M7" s="31">
-        <f t="shared" ref="M7:N7" si="1">F43</f>
-        <v>51.800000000000004</v>
-      </c>
-      <c r="N7" s="31">
+        <f t="shared" ref="M7:N7" si="1">F45</f>
+        <v>36.329000000000008</v>
+      </c>
+      <c r="N7" s="70">
         <f t="shared" si="1"/>
-        <v>82.17</v>
+        <v>55.140999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="67"/>
+      <c r="B8" s="77"/>
       <c r="G8" s="26"/>
-      <c r="K8" t="str">
-        <f>B45</f>
+      <c r="K8" s="69" t="str">
+        <f>B47</f>
         <v>-12V</v>
       </c>
       <c r="L8" s="31">
-        <f>E56</f>
-        <v>10.504</v>
+        <f>E58</f>
+        <v>9.6920000000000002</v>
       </c>
       <c r="M8" s="31">
-        <f t="shared" ref="M8:N8" si="2">F56</f>
-        <v>10.8</v>
-      </c>
-      <c r="N8" s="31">
+        <f t="shared" ref="M8:N8" si="2">F58</f>
+        <v>10</v>
+      </c>
+      <c r="N8" s="70">
         <f t="shared" si="2"/>
-        <v>12.3</v>
+        <v>10.012</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="67"/>
+      <c r="B9" s="77"/>
       <c r="G9" s="26"/>
-      <c r="K9" t="str">
-        <f>B58</f>
+      <c r="K9" s="69" t="str">
+        <f>B60</f>
         <v>+5V_A</v>
       </c>
       <c r="L9" s="31">
-        <f>E63</f>
+        <f>E65</f>
         <v>1.10012</v>
       </c>
       <c r="M9" s="31">
-        <f>F63</f>
+        <f>F65</f>
         <v>1.8599999999999999</v>
       </c>
-      <c r="N9" s="31">
-        <f>G63</f>
+      <c r="N9" s="70">
+        <f>G65</f>
         <v>2.37</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="67"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="21" t="s">
         <v>116</v>
       </c>
@@ -3637,96 +3832,109 @@
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="28"/>
-      <c r="K10" t="str">
-        <f>B65</f>
+      <c r="K10" s="71" t="str">
+        <f>B67</f>
         <v>+1V8_A</v>
       </c>
-      <c r="L10" s="31">
-        <f>E68</f>
+      <c r="L10" s="18">
+        <f>E70</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="M10" s="31">
-        <f>F68</f>
+      <c r="M10" s="18">
+        <f>F70</f>
         <v>1.98</v>
       </c>
-      <c r="N10" s="31">
-        <f>G68</f>
+      <c r="N10" s="72">
+        <f>G70</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="67"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="9" t="s">
-        <v>269</v>
+        <v>307</v>
       </c>
       <c r="E11" s="16">
-        <f>(E43+E53)*15/_RAIL_5V/EFF_12V_BOOST</f>
-        <v>216.15</v>
+        <f>E45*15/_RAIL_5V/EFF_12V_BOOST</f>
+        <v>131.84294999999997</v>
       </c>
       <c r="F11" s="16">
-        <f>(F43+F53)*15/_RAIL_5V/EFF_12V_BOOST</f>
-        <v>216.75000000000003</v>
+        <f>F45*15/_RAIL_5V/EFF_12V_BOOST</f>
+        <v>136.23375000000004</v>
       </c>
       <c r="G11" s="26">
-        <f>(G43+G53)*15/_RAIL_5V/EFF_12V_BOOST</f>
-        <v>332.51249999999999</v>
+        <f>G45*15/_RAIL_5V/EFF_12V_BOOST</f>
+        <v>206.77874999999995</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="67"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="9" t="s">
-        <v>136</v>
+        <v>308</v>
       </c>
       <c r="E12" s="16">
+        <f>E58*15/_RAIL_5V/EFF_12V_BOOST</f>
+        <v>36.344999999999999</v>
+      </c>
+      <c r="F12" s="16">
+        <f>F58*15/_RAIL_5V/EFF_12V_BOOST</f>
+        <v>37.5</v>
+      </c>
+      <c r="G12" s="26">
+        <f>G58*15/_RAIL_5V/EFF_12V_BOOST</f>
+        <v>37.545000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="77"/>
+      <c r="C13" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="16">
         <f>E30</f>
-        <v>2.8528599999999997</v>
-      </c>
-      <c r="F12" s="16">
+        <v>4.1608599999999996</v>
+      </c>
+      <c r="F13" s="16">
         <f>F30</f>
-        <v>9.0220000000000002</v>
-      </c>
-      <c r="G12" s="26">
+        <v>11.328000000000001</v>
+      </c>
+      <c r="G13" s="26">
         <f>G30</f>
-        <v>11.067</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="67"/>
-      <c r="C13" s="9"/>
-      <c r="G13" s="26"/>
+        <v>12.381999999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="67"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="9"/>
       <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="68"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="22" t="s">
         <v>121</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="29">
         <f>SUM(E5:E13)</f>
-        <v>321.00286</v>
+        <v>263.89880999999997</v>
       </c>
       <c r="F15" s="29">
         <f>SUM(F5:F13)</f>
-        <v>327.77199999999999</v>
+        <v>286.62175000000002</v>
       </c>
       <c r="G15" s="30">
         <f>SUM(G5:G13)</f>
-        <v>446.5795</v>
+        <v>368.49974999999995</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="65"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="76" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="20" t="s">
@@ -3738,9 +3946,9 @@
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="67"/>
+      <c r="B18" s="77"/>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E18" s="16">
         <f>3*0.00012</f>
@@ -3756,27 +3964,27 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="67"/>
+      <c r="B19" s="77"/>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>312</v>
       </c>
       <c r="E19" s="16">
-        <f>3*0.002</f>
-        <v>6.0000000000000001E-3</v>
+        <f>4*0.002</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F19" s="16">
         <f>G19</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G19" s="26">
-        <f>3*1</f>
-        <v>3</v>
+        <f>4*1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="67"/>
+      <c r="B20" s="77"/>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E20" s="16">
         <f>24*3.3/100000*1000</f>
@@ -3792,24 +4000,24 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="67"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E21" s="16">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="F21" s="16">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="G21" s="26">
-        <v>3</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="67"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E22" s="16">
         <v>0.05</v>
@@ -3822,19 +4030,30 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="67"/>
-      <c r="G23" s="26"/>
+      <c r="B23" s="77"/>
+      <c r="C23" t="s">
+        <v>311</v>
+      </c>
+      <c r="E23" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F23" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G23" s="26">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="67"/>
+      <c r="B24" s="77"/>
       <c r="G24" s="26"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="67"/>
+      <c r="B25" s="77"/>
       <c r="G25" s="26"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="67"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="21" t="s">
         <v>116</v>
       </c>
@@ -3844,55 +4063,55 @@
       <c r="G26" s="28"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="67"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E27" s="16">
-        <f>E68</f>
+        <f>E70</f>
         <v>4.5000000000000005E-3</v>
       </c>
       <c r="F27" s="16">
-        <f>F68</f>
+        <f>F70</f>
         <v>1.98</v>
       </c>
       <c r="G27" s="26">
-        <f>G68</f>
+        <f>G70</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="67"/>
+      <c r="B28" s="77"/>
       <c r="G28" s="26"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="67"/>
+      <c r="B29" s="77"/>
       <c r="G29" s="26"/>
     </row>
     <row r="30" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="68"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="22" t="s">
         <v>121</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="29">
         <f>SUM(E18:E29)</f>
-        <v>2.8528599999999997</v>
+        <v>4.1608599999999996</v>
       </c>
       <c r="F30" s="29">
         <f>SUM(F18:F29)</f>
-        <v>9.0220000000000002</v>
+        <v>11.328000000000001</v>
       </c>
       <c r="G30" s="30">
         <f>SUM(G18:G29)</f>
-        <v>11.067</v>
+        <v>12.381999999999998</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="65"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="76" t="s">
         <v>118</v>
       </c>
       <c r="C32" s="20" t="s">
@@ -3903,8 +4122,8 @@
       <c r="F32" s="24"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="67"/>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="77"/>
       <c r="C33" t="s">
         <v>127</v>
       </c>
@@ -3918,28 +4137,40 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="67"/>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B34" s="77"/>
       <c r="C34" t="s">
+        <v>318</v>
+      </c>
+      <c r="E34" s="16">
+        <f>8*3.2</f>
+        <v>25.6</v>
+      </c>
+      <c r="F34" s="16">
+        <f>8*3.2</f>
+        <v>25.6</v>
+      </c>
+      <c r="G34" s="26">
+        <f>8*4.6</f>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="L34" t="s">
+        <v>112</v>
+      </c>
+      <c r="M34" t="s">
+        <v>113</v>
+      </c>
+      <c r="N34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B35" s="77"/>
+      <c r="C35" t="s">
         <v>128</v>
-      </c>
-      <c r="E34" s="16">
-        <f>6*7</f>
-        <v>42</v>
-      </c>
-      <c r="F34" s="16">
-        <f>6*7</f>
-        <v>42</v>
-      </c>
-      <c r="G34" s="26">
-        <f>9*7</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="67"/>
-      <c r="C35" t="s">
-        <v>129</v>
       </c>
       <c r="E35" s="16">
         <f>0.01*4</f>
@@ -3953,11 +4184,26 @@
         <f>0.075*4</f>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="67"/>
+      <c r="K35" t="s">
+        <v>315</v>
+      </c>
+      <c r="L35">
+        <v>6</v>
+      </c>
+      <c r="M35">
+        <v>6</v>
+      </c>
+      <c r="N35">
+        <v>9</v>
+      </c>
+      <c r="O35" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B36" s="77"/>
       <c r="C36" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E36" s="16">
         <v>5</v>
@@ -3968,11 +4214,23 @@
       <c r="G36" s="26">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="67"/>
+      <c r="K36" s="73" t="s">
+        <v>316</v>
+      </c>
+      <c r="L36" s="74">
+        <v>3.2</v>
+      </c>
+      <c r="M36" s="74">
+        <v>3.2</v>
+      </c>
+      <c r="N36" s="75">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B37" s="77"/>
       <c r="C37" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E37" s="16">
         <v>2</v>
@@ -3984,360 +4242,392 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="67"/>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B38" s="77"/>
       <c r="C38" s="9" t="s">
-        <v>144</v>
+        <v>319</v>
       </c>
       <c r="E38" s="16">
-        <v>2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F38" s="16">
-        <v>2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G38" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="67"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B39" s="77"/>
+      <c r="C39" s="9"/>
       <c r="G39" s="26"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="67"/>
-      <c r="C40" s="21" t="s">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B40" s="77"/>
+      <c r="G40" s="26"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B41" s="77"/>
+      <c r="C41" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="21"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="28"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="67"/>
-      <c r="C41" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="67"/>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="68"/>
-      <c r="C43" s="22" t="s">
+      <c r="D41" s="21"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B42" s="77"/>
+      <c r="C42" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E42" s="16">
+        <v>0.748</v>
+      </c>
+      <c r="F42" s="16">
+        <v>0.999</v>
+      </c>
+      <c r="G42" s="26">
+        <v>1.7010000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B43" s="77"/>
+      <c r="C43" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="E43" s="16">
+        <f>E65</f>
+        <v>1.10012</v>
+      </c>
+      <c r="F43" s="16">
+        <f>F65</f>
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="G43" s="26">
+        <f>G65</f>
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B44" s="77"/>
+      <c r="G44" s="26"/>
+    </row>
+    <row r="45" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="78"/>
+      <c r="C45" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="29">
-        <f>SUM(E33:E42)</f>
-        <v>51.64</v>
-      </c>
-      <c r="F43" s="29">
-        <f>SUM(F33:F42)</f>
-        <v>51.800000000000004</v>
-      </c>
-      <c r="G43" s="30">
-        <f>SUM(G33:G42)</f>
-        <v>82.17</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="65"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="66" t="s">
+      <c r="D45" s="23"/>
+      <c r="E45" s="29">
+        <f>SUM(E33:E44)</f>
+        <v>35.158119999999997</v>
+      </c>
+      <c r="F45" s="29">
+        <f>SUM(F33:F44)</f>
+        <v>36.329000000000008</v>
+      </c>
+      <c r="G45" s="30">
+        <f>SUM(G33:G44)</f>
+        <v>55.140999999999991</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="65"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C47" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="67"/>
-      <c r="C46" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" s="16">
+      <c r="D47" s="20"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="25"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48" s="77"/>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="16">
         <f>4*0.001</f>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F46" s="16">
+      <c r="F48" s="16">
         <f>4*0.075</f>
         <v>0.3</v>
       </c>
-      <c r="G46" s="26">
-        <f>F46</f>
+      <c r="G48" s="26">
+        <f>F48</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="67"/>
-      <c r="C47" t="s">
-        <v>268</v>
-      </c>
-      <c r="E47" s="16">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="77"/>
+      <c r="C49" t="s">
+        <v>262</v>
+      </c>
+      <c r="E49" s="16">
         <v>2.5</v>
       </c>
-      <c r="F47" s="16">
+      <c r="F49" s="16">
         <v>2.5</v>
       </c>
-      <c r="G47" s="26">
+      <c r="G49" s="26">
         <v>2.5</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="67"/>
-      <c r="C48" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="16">
-        <v>2</v>
-      </c>
-      <c r="F48" s="16">
-        <v>2</v>
-      </c>
-      <c r="G48" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="67"/>
-      <c r="C49" s="9"/>
-      <c r="G49" s="26"/>
-    </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="67"/>
-      <c r="G50" s="26"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E50" s="16">
+        <v>1.1879999999999999</v>
+      </c>
+      <c r="F50" s="16">
+        <v>1.2</v>
+      </c>
+      <c r="G50" s="26">
+        <v>1.212</v>
+      </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="67"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="9"/>
       <c r="G51" s="26"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="67"/>
-      <c r="C52" s="21" t="s">
+      <c r="B52" s="77"/>
+      <c r="G52" s="26"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="77"/>
+      <c r="G53" s="26"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="77"/>
+      <c r="C54" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="28"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="67"/>
-      <c r="C53" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E53" s="16">
+      <c r="D54" s="21"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="28"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="77"/>
+      <c r="C55" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E55" s="16">
         <v>6</v>
       </c>
-      <c r="F53" s="16">
+      <c r="F55" s="16">
         <v>6</v>
       </c>
-      <c r="G53" s="26">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="67"/>
-      <c r="G54" s="26"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="67"/>
-      <c r="G55" s="26"/>
-    </row>
-    <row r="56" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="68"/>
-      <c r="C56" s="22" t="s">
+      <c r="G55" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="77"/>
+      <c r="G56" s="26"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="77"/>
+      <c r="G57" s="26"/>
+    </row>
+    <row r="58" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="78"/>
+      <c r="C58" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="29">
-        <f>SUM(E46:E55)</f>
-        <v>10.504</v>
-      </c>
-      <c r="F56" s="29">
-        <f>SUM(F46:F55)</f>
-        <v>10.8</v>
-      </c>
-      <c r="G56" s="30">
-        <f>SUM(G46:G55)</f>
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="65"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="66" t="s">
+      <c r="D58" s="23"/>
+      <c r="E58" s="29">
+        <f>SUM(E48:E57)</f>
+        <v>9.6920000000000002</v>
+      </c>
+      <c r="F58" s="29">
+        <f>SUM(F48:F57)</f>
+        <v>10</v>
+      </c>
+      <c r="G58" s="30">
+        <f>SUM(G48:G57)</f>
+        <v>10.012</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="65"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C60" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="25"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="67"/>
-      <c r="C59" t="s">
-        <v>131</v>
-      </c>
-      <c r="E59" s="16">
+      <c r="D60" s="20"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="25"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="77"/>
+      <c r="C61" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="16">
         <f>3*0.00004</f>
         <v>1.2000000000000002E-4</v>
       </c>
-      <c r="F59" s="16">
+      <c r="F61" s="16">
         <f>3*0.22</f>
         <v>0.66</v>
       </c>
-      <c r="G59" s="26">
+      <c r="G61" s="26">
         <f>3*0.29</f>
         <v>0.86999999999999988</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="67"/>
-      <c r="C60" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E60" s="40">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="77"/>
+      <c r="C62" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="40">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F60" s="40">
+      <c r="F62" s="40">
         <v>1.2</v>
       </c>
-      <c r="G60" s="63">
+      <c r="G62" s="63">
         <v>1.5</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="67"/>
-      <c r="G61" s="26"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="67"/>
-      <c r="G62" s="26"/>
-    </row>
-    <row r="63" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="68"/>
-      <c r="C63" s="22" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="77"/>
+      <c r="G63" s="26"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="77"/>
+      <c r="G64" s="26"/>
+    </row>
+    <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="78"/>
+      <c r="C65" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="29">
-        <f>SUM(E59:E62)</f>
+      <c r="D65" s="23"/>
+      <c r="E65" s="29">
+        <f>SUM(E61:E64)</f>
         <v>1.10012</v>
       </c>
-      <c r="F63" s="29">
-        <f>SUM(F59:F62)</f>
+      <c r="F65" s="29">
+        <f>SUM(F61:F64)</f>
         <v>1.8599999999999999</v>
       </c>
-      <c r="G63" s="30">
-        <f>SUM(G59:G62)</f>
+      <c r="G65" s="30">
+        <f>SUM(G61:G64)</f>
         <v>2.37</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B65" s="66" t="s">
+    <row r="66" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C67" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="25"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B66" s="67"/>
-      <c r="C66" t="s">
-        <v>132</v>
-      </c>
-      <c r="E66" s="16">
+      <c r="D67" s="20"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="25"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="77"/>
+      <c r="C68" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" s="16">
         <f>3*0.0015</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="F66" s="16">
+      <c r="F68" s="16">
         <f>3*0.66</f>
         <v>1.98</v>
       </c>
-      <c r="G66" s="26">
+      <c r="G68" s="26">
         <f>3*0.9</f>
         <v>2.7</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="67"/>
-      <c r="C67" s="9"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67" s="32"/>
-    </row>
-    <row r="68" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="68"/>
-      <c r="C68" s="22" t="s">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="77"/>
+      <c r="C69" s="9"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69" s="32"/>
+    </row>
+    <row r="70" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="78"/>
+      <c r="C70" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D68" s="23"/>
-      <c r="E68" s="29">
-        <f>SUM(E66:E67)</f>
+      <c r="D70" s="23"/>
+      <c r="E70" s="29">
+        <f>SUM(E68:E69)</f>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="F68" s="29">
-        <f>SUM(F66:F67)</f>
+      <c r="F70" s="29">
+        <f>SUM(F68:F69)</f>
         <v>1.98</v>
       </c>
-      <c r="G68" s="30">
-        <f>SUM(G66:G67)</f>
+      <c r="G70" s="30">
+        <f>SUM(G68:G69)</f>
         <v>2.7</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B69" s="65"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B70" s="65"/>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="65"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" s="65"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B73" s="65"/>
-    </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" s="65"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" s="65"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76" s="65"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B77" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B4:B15"/>
     <mergeCell ref="B17:B30"/>
-    <mergeCell ref="B32:B43"/>
-    <mergeCell ref="B45:B56"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B32:B45"/>
+    <mergeCell ref="B47:B58"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B60:B65"/>
   </mergeCells>
   <conditionalFormatting sqref="E15:G15">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>499.99</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4914,7 +5204,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -5146,7 +5436,7 @@
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -5157,7 +5447,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B25" s="4">
         <f>(B24-1.76)/6.02</f>
@@ -5238,12 +5528,12 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B31" s="4">
         <f>(B30-1.76)/6.02</f>
@@ -5267,7 +5557,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5280,10 +5570,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B38" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -5300,8 +5590,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5320,13 +5610,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -5374,11 +5664,11 @@
         <v>3</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="79" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -5410,7 +5700,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="70"/>
+      <c r="A9" s="80"/>
       <c r="B9" t="s">
         <v>104</v>
       </c>
@@ -5433,7 +5723,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="70"/>
+      <c r="A10" s="80"/>
       <c r="B10" t="s">
         <v>105</v>
       </c>
@@ -5454,7 +5744,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="13" t="s">
         <v>106</v>
       </c>
@@ -5478,7 +5768,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="82" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -5510,7 +5800,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="73"/>
+      <c r="A13" s="83"/>
       <c r="B13" t="s">
         <v>104</v>
       </c>
@@ -5534,7 +5824,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="73"/>
+      <c r="A14" s="83"/>
       <c r="B14" t="s">
         <v>105</v>
       </c>
@@ -5555,7 +5845,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="74"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="13" t="s">
         <v>106</v>
       </c>
@@ -5579,7 +5869,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="85" t="s">
         <v>109</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -5611,7 +5901,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="76"/>
+      <c r="A17" s="86"/>
       <c r="B17" t="s">
         <v>104</v>
       </c>
@@ -5635,7 +5925,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="76"/>
+      <c r="A18" s="86"/>
       <c r="B18" t="s">
         <v>105</v>
       </c>
@@ -5656,7 +5946,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
+      <c r="A19" s="87"/>
       <c r="B19" s="13" t="s">
         <v>106</v>
       </c>
@@ -5680,7 +5970,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="88" t="s">
         <v>110</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -5712,7 +6002,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+      <c r="A21" s="89"/>
       <c r="B21" t="s">
         <v>104</v>
       </c>
@@ -5736,7 +6026,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="79"/>
+      <c r="A22" s="89"/>
       <c r="B22" t="s">
         <v>105</v>
       </c>
@@ -5757,7 +6047,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
+      <c r="A23" s="90"/>
       <c r="B23" s="13" t="s">
         <v>106</v>
       </c>
@@ -5816,7 +6106,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -5847,35 +6137,35 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B5">
         <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G5">
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -5884,10 +6174,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G6">
         <v>-15</v>
@@ -5907,7 +6197,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
         <v>100</v>
@@ -5921,44 +6211,44 @@
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B8" s="45">
         <v>47.5</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G8" s="45">
         <v>47.5</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <f>B8*(B6/B7-1)</f>
         <v>539.88664468260504</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F9" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G9">
         <f>-1*G8*G6/G7</f>
         <v>587.38664468260504</v>
       </c>
       <c r="H9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -5970,21 +6260,21 @@
         <v>536</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G11" s="45">
         <v>576</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B12">
         <f>(1+B11/B8)*B7</f>
@@ -5994,7 +6284,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G12">
         <f>-G11/G8*G7</f>
@@ -6006,15 +6296,15 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -6023,7 +6313,7 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G23">
         <v>5</v>
@@ -6034,77 +6324,77 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B24">
         <v>0.08</v>
       </c>
       <c r="C24" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D24" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F24" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G24">
         <v>0.01</v>
       </c>
       <c r="H24" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B25">
         <f>B6/(B23*0.64)*B24</f>
         <v>0.375</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F25" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G25">
         <f>(G23-G6)/(G23*0.64)*G24</f>
         <v>6.25E-2</v>
       </c>
       <c r="H25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B26">
         <f>0.2*B25</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="C26" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" t="s">
         <v>184</v>
-      </c>
-      <c r="F26" t="s">
-        <v>189</v>
       </c>
       <c r="G26">
         <f>0.2*G25</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="H26" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B27">
         <v>1.25</v>
@@ -6113,7 +6403,7 @@
         <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G27">
         <v>1.25</v>
@@ -6124,43 +6414,43 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B28" s="47">
         <f>B23*(B6-B23)/(B26*B27*B6)</f>
         <v>35.55555555555555</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F28" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G28" s="48">
         <f>G23*G6/(G26*G27*(G6-G23))</f>
         <v>240</v>
       </c>
       <c r="H28" s="48" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I28" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B32">
         <v>5.0000000000000001E-3</v>
@@ -6169,7 +6459,7 @@
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G32">
         <v>5.0000000000000001E-3</v>
@@ -6180,29 +6470,29 @@
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B33" s="49">
         <f>B24*(B6-B23)/(B27*B32*B6)</f>
         <v>8.5333333333333332</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F33" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G33" s="45">
         <f>G24*G6/(G27*G32*(G6-G23))</f>
         <v>1.2</v>
       </c>
       <c r="H33" s="46" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B34">
         <v>0.01</v>
@@ -6211,7 +6501,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G34">
         <v>0.01</v>
@@ -6222,7 +6512,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B35">
         <f>B24*B34</f>
@@ -6232,7 +6522,7 @@
         <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G35">
         <f>G24*G34</f>
@@ -6244,52 +6534,52 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B39" s="50">
         <f>0.0000068/(B11*1000)</f>
         <v>1.2686567164179104E-11</v>
       </c>
       <c r="C39" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F39" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G39" s="50">
         <f>0.0000075/(G11*1000)</f>
         <v>1.3020833333333334E-11</v>
       </c>
       <c r="H39" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B40">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F40" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G40">
         <v>13</v>
       </c>
       <c r="H40" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -6306,8 +6596,8 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6319,7 +6609,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6327,7 +6617,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>96</v>
@@ -6347,12 +6637,12 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="58" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B5" s="59">
         <v>0.01</v>
@@ -6369,12 +6659,12 @@
         <v>541.36</v>
       </c>
       <c r="F5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B6" s="59">
         <v>0.01</v>
@@ -6391,7 +6681,7 @@
         <v>47.975000000000001</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6416,7 +6706,7 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -6439,12 +6729,12 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="58" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B11" s="59">
         <v>0.01</v>
@@ -6461,12 +6751,12 @@
         <v>581.76</v>
       </c>
       <c r="F11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B12" s="59">
         <v>0.01</v>
@@ -6483,7 +6773,7 @@
         <v>47.975000000000001</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6508,7 +6798,7 @@
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
@@ -6531,12 +6821,12 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="58" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s">
         <v>63</v>
@@ -6556,7 +6846,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C18">
         <f>12+C17</f>
@@ -6574,30 +6864,30 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C19" s="59">
-        <v>-0.05</v>
+        <v>-0.03</v>
       </c>
       <c r="D19" s="59">
         <v>0</v>
       </c>
       <c r="E19" s="59">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C20" s="45">
         <f>12*(1+C19)</f>
-        <v>11.399999999999999</v>
+        <v>11.64</v>
       </c>
       <c r="D20" s="60">
         <f>12*(1+D19)</f>
@@ -6605,7 +6895,7 @@
       </c>
       <c r="E20" s="60">
         <f>12*(1+E19)</f>
-        <v>12.600000000000001</v>
+        <v>12.36</v>
       </c>
       <c r="F20" s="46" t="s">
         <v>5</v>
@@ -6613,12 +6903,12 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="58" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B23" t="s">
         <v>63</v>
@@ -6638,7 +6928,7 @@
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C24">
         <f>-12-C23</f>
@@ -6656,12 +6946,12 @@
         <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C25" s="45">
         <v>-11.4</v>
@@ -6676,17 +6966,17 @@
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="58" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C28">
         <v>0.35</v>
@@ -6703,7 +6993,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C29">
         <f>1.8+C28</f>
@@ -6721,12 +7011,12 @@
         <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B30" t="s">
         <v>63</v>
@@ -6743,7 +7033,7 @@
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C31" s="45">
         <f>1.8*(1+C30)</f>
@@ -6774,8 +7064,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6787,7 +7077,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6804,7 +7094,7 @@
         <v>97</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>3</v>
@@ -6815,7 +7105,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -6838,7 +7128,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -6856,12 +7146,12 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -6889,7 +7179,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -6907,12 +7197,12 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
@@ -6937,7 +7227,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C11" s="16">
         <f>C8-E9</f>
@@ -6957,7 +7247,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C12" s="37">
         <f>C11/E6</f>
@@ -6972,7 +7262,7 @@
         <v>7.1041475022997247</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -6982,7 +7272,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
@@ -6994,10 +7284,10 @@
       </c>
       <c r="E14" s="16"/>
       <c r="F14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" t="s">
         <v>157</v>
-      </c>
-      <c r="G14" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7007,7 +7297,7 @@
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="41" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B16" s="42">
         <v>0.01</v>
@@ -7024,12 +7314,12 @@
         <v>4.2622</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C17" s="31">
         <f>C11/E16-E4</f>
@@ -7047,7 +7337,7 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -7094,12 +7384,12 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -7108,12 +7398,12 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -7122,12 +7412,12 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7138,7 +7428,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -7191,7 +7481,7 @@
         <v>1290322.5806451612</v>
       </c>
       <c r="D13" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -7335,9 +7625,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4773A798-633B-4D8D-9FC8-9ECE55BCD182}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -7346,268 +7636,462 @@
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" t="s">
+        <v>284</v>
+      </c>
+      <c r="G7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>249</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
+      <c r="F10" t="s">
+        <v>248</v>
+      </c>
+      <c r="G10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F11" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" t="s">
+        <v>250</v>
+      </c>
+      <c r="G12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>261</v>
+      </c>
+      <c r="F13" t="s">
+        <v>285</v>
+      </c>
+      <c r="G13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" t="s">
+        <v>252</v>
+      </c>
+      <c r="G14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" t="s">
+        <v>260</v>
+      </c>
+      <c r="F15" t="s">
+        <v>286</v>
+      </c>
+      <c r="G15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" t="s">
+        <v>287</v>
+      </c>
+      <c r="G16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>288</v>
+      </c>
+      <c r="G17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" t="s">
+        <v>289</v>
+      </c>
+      <c r="G18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F19" t="s">
+        <v>253</v>
+      </c>
+      <c r="G19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>250</v>
-      </c>
-      <c r="B4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>251</v>
-      </c>
-      <c r="B5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B8" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>256</v>
-      </c>
-      <c r="B10" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B20" t="s">
+        <v>260</v>
+      </c>
+      <c r="F20" t="s">
         <v>257</v>
       </c>
-      <c r="B11" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>258</v>
-      </c>
-      <c r="B12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
-        <v>259</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>265</v>
-      </c>
-      <c r="C13" s="62" t="s">
+      <c r="G20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>266</v>
+      </c>
+      <c r="B21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" t="s">
+        <v>290</v>
+      </c>
+      <c r="G21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B22" t="s">
         <v>260</v>
       </c>
-      <c r="B14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>261</v>
-      </c>
-      <c r="B15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>262</v>
-      </c>
-      <c r="B16" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F23" t="s">
+        <v>292</v>
+      </c>
+      <c r="G23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>269</v>
+      </c>
+      <c r="B24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F24" t="s">
+        <v>293</v>
+      </c>
+      <c r="G24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>270</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>271</v>
       </c>
-      <c r="B19" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>272</v>
       </c>
-      <c r="B20" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B27" t="s">
+        <v>260</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" t="s">
+        <v>260</v>
+      </c>
+      <c r="F28" t="s">
+        <v>295</v>
+      </c>
+      <c r="G28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>273</v>
       </c>
-      <c r="B21" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>274</v>
-      </c>
-      <c r="B22" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B29" t="s">
+        <v>260</v>
+      </c>
+      <c r="F29" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>275</v>
       </c>
-      <c r="B23" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B30" t="s">
+        <v>260</v>
+      </c>
+      <c r="F30" t="s">
+        <v>299</v>
+      </c>
+      <c r="G30" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>276</v>
       </c>
-      <c r="B24" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>277</v>
-      </c>
-      <c r="B25" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>278</v>
-      </c>
-      <c r="B26" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>279</v>
-      </c>
-      <c r="B27" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>280</v>
-      </c>
-      <c r="B28" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>282</v>
-      </c>
-      <c r="B29" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>281</v>
-      </c>
-      <c r="B30" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>283</v>
-      </c>
       <c r="B31" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="F31" t="s">
+        <v>301</v>
+      </c>
+      <c r="G31" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>260</v>
+      </c>
+      <c r="F32" t="s">
+        <v>302</v>
+      </c>
+      <c r="G32" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>304</v>
+      </c>
+      <c r="G33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>305</v>
+      </c>
+      <c r="G34" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B160">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="In Progress">
+  <conditionalFormatting sqref="B2:B159">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
starting firmware for DAQ device by refactoring eval board code
</commit_message>
<xml_diff>
--- a/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
+++ b/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\0 Documentation\1 Design Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCEFB1E-66AD-4605-BF80-8D5390567D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF1D3EC-0CAD-4BF1-814B-2C9F81384495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="3" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="5" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="6" r:id="rId1"/>
@@ -4625,7 +4625,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="46" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
@@ -5590,8 +5590,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6596,8 +6596,8 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6671,14 +6671,14 @@
       </c>
       <c r="C6">
         <f>(1-B6)*D6</f>
-        <v>47.024999999999999</v>
+        <v>48.213000000000001</v>
       </c>
       <c r="D6">
-        <v>47.5</v>
+        <v>48.7</v>
       </c>
       <c r="E6">
         <f>(1+B6)*D6</f>
-        <v>47.975000000000001</v>
+        <v>49.187000000000005</v>
       </c>
       <c r="F6" t="s">
         <v>152</v>
@@ -6713,15 +6713,15 @@
       </c>
       <c r="C8" s="45">
         <f>C7*(C5/E6+1)</f>
-        <v>14.472912975508075</v>
+        <v>14.145859678370298</v>
       </c>
       <c r="D8" s="60">
         <f>D7*(D5/D6+1)</f>
-        <v>14.900747368421053</v>
+        <v>14.563472279260779</v>
       </c>
       <c r="E8" s="60">
         <f>E7*(E5/C6+1)</f>
-        <v>15.327413609782033</v>
+        <v>14.979920871963994</v>
       </c>
       <c r="F8" s="46" t="s">
         <v>5</v>
@@ -6763,14 +6763,14 @@
       </c>
       <c r="C12">
         <f>(1-B12)*D12</f>
-        <v>47.024999999999999</v>
+        <v>48.213000000000001</v>
       </c>
       <c r="D12">
-        <v>47.5</v>
+        <v>48.7</v>
       </c>
       <c r="E12">
         <f>(1+B12)*D12</f>
-        <v>47.975000000000001</v>
+        <v>49.187000000000005</v>
       </c>
       <c r="F12" t="s">
         <v>152</v>
@@ -6805,15 +6805,15 @@
       </c>
       <c r="C14" s="45">
         <f>-E13*E11/C12</f>
-        <v>-15.15483253588517</v>
+        <v>-14.781407504200113</v>
       </c>
       <c r="D14" s="60">
         <f>-D13*D11/D12</f>
-        <v>-14.70922105263158</v>
+        <v>-14.346776180698154</v>
       </c>
       <c r="E14" s="60">
         <f>-C13*C11/E12</f>
-        <v>-14.263428869202709</v>
+        <v>-13.911968609591964</v>
       </c>
       <c r="F14" s="46" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
cleaned up repo, delete unnecessary files/data
</commit_message>
<xml_diff>
--- a/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
+++ b/0 Documentation/1 Design Calculations/Hardware Design Calculations.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\0 Documentation\1 Design Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF1D3EC-0CAD-4BF1-814B-2C9F81384495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755A817F-5553-408E-AE34-277D3E2B4DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="1" activeTab="5" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="833" firstSheet="2" activeTab="8" xr2:uid="{332224D6-7097-403A-AE45-EBC3D80EB06D}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="6" r:id="rId1"/>
     <sheet name="Digital Input Protection" sheetId="1" r:id="rId2"/>
     <sheet name="ADC Resolution" sheetId="2" r:id="rId3"/>
-    <sheet name="ADC Tolerance" sheetId="5" r:id="rId4"/>
+    <sheet name="Non-Inv Gain Tolerance" sheetId="5" r:id="rId4"/>
     <sheet name="TPS65131 Calcs" sheetId="8" r:id="rId5"/>
     <sheet name="Pwr Mgmt Tolerances" sheetId="9" r:id="rId6"/>
     <sheet name="5V Precision Ref Biasing" sheetId="7" r:id="rId7"/>
     <sheet name="ADC SPI Bandwidth" sheetId="3" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
-    <sheet name="High-Speed AIN Filtering" sheetId="4" r:id="rId10"/>
+    <sheet name="dB to V" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_RAIL_12V">12</definedName>
@@ -88,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="268">
   <si>
     <t>Digital Input Protection</t>
   </si>
@@ -180,9 +179,6 @@
     <t>dB</t>
   </si>
   <si>
-    <t>ADC SPI Bandwidth</t>
-  </si>
-  <si>
     <t>SPI clock frequency</t>
   </si>
   <si>
@@ -276,9 +272,6 @@
     <t>Input voltage at which Pdiss of R1 is 0.5W</t>
   </si>
   <si>
-    <t>High-Speed Analog Input Filtering</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -375,9 +368,6 @@
     <t>14-bit SAR 1Msps SPI single-ended</t>
   </si>
   <si>
-    <t>ADC Tolerance Calculations</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
@@ -714,27 +704,15 @@
     <t>Calculations are estimation for the MCP33151-10</t>
   </si>
   <si>
-    <t>Sent in groups of 8 bits</t>
-  </si>
-  <si>
     <t>Dead time between 8-bit bursts</t>
   </si>
   <si>
     <t>ADC data bits</t>
   </si>
   <si>
-    <t>Dead time from CS low to start</t>
-  </si>
-  <si>
     <t>Dead time from end to CS high</t>
   </si>
   <si>
-    <t>number of equivalent clock cycles</t>
-  </si>
-  <si>
-    <t>So theoretically we can hit 1Msps if Teensy is fast enough</t>
-  </si>
-  <si>
     <t>Resolution</t>
   </si>
   <si>
@@ -819,195 +797,9 @@
     <t>Min. 60uA. Cannot exceed 15mA.</t>
   </si>
   <si>
-    <t>Mid-Project Report Progress</t>
-  </si>
-  <si>
-    <t>Abstract</t>
-  </si>
-  <si>
-    <t>List of Abbreviations</t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>Background</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Plan for next semseter</t>
-  </si>
-  <si>
-    <t>Impact on Society and Environment</t>
-  </si>
-  <si>
-    <t>Conclusion</t>
-  </si>
-  <si>
-    <t>A1-Perfboard</t>
-  </si>
-  <si>
-    <t>A2-Eval board</t>
-  </si>
-  <si>
-    <t>A3-Design calculations</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Done?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>removed :)</t>
-  </si>
-  <si>
     <t>DG409 dual 4:1 mux x 5</t>
   </si>
   <si>
-    <t>Review Checklist</t>
-  </si>
-  <si>
-    <t>Tense -- past vs present</t>
-  </si>
-  <si>
-    <t>Capitalization on figures and tables captions</t>
-  </si>
-  <si>
-    <t>Abbreviations first instance</t>
-  </si>
-  <si>
-    <t>Requirements -- bolded shalls</t>
-  </si>
-  <si>
-    <t>Figures -- text readable</t>
-  </si>
-  <si>
-    <t>SI unitx used everywhere</t>
-  </si>
-  <si>
-    <t>No more todos left</t>
-  </si>
-  <si>
-    <t>No watermark</t>
-  </si>
-  <si>
-    <t>All abbreviations are in the list</t>
-  </si>
-  <si>
-    <t>All tables are referenced in the text</t>
-  </si>
-  <si>
-    <t>All figures are referenced in the text</t>
-  </si>
-  <si>
-    <t>Sections make sense, no further division needed</t>
-  </si>
-  <si>
-    <t>All sections in rubric are present in report</t>
-  </si>
-  <si>
-    <t>skipping, looked good on two readthroughs</t>
-  </si>
-  <si>
-    <t>update main block diagram resolution</t>
-  </si>
-  <si>
-    <t>Rubric Sections</t>
-  </si>
-  <si>
-    <t>Present?</t>
-  </si>
-  <si>
-    <t>Title page</t>
-  </si>
-  <si>
-    <t>Acknowledgements</t>
-  </si>
-  <si>
-    <t>Table of Contents</t>
-  </si>
-  <si>
-    <t>List of abbreviations</t>
-  </si>
-  <si>
-    <t>Plan for Next Semester</t>
-  </si>
-  <si>
-    <t>use of non-renewable resources</t>
-  </si>
-  <si>
-    <t>environmental benefits</t>
-  </si>
-  <si>
-    <t>safety and risk</t>
-  </si>
-  <si>
-    <t>benefits to society</t>
-  </si>
-  <si>
-    <t>Appendices</t>
-  </si>
-  <si>
-    <t>Check rubric grading elements</t>
-  </si>
-  <si>
-    <t>1 inch margins</t>
-  </si>
-  <si>
-    <t>11pt font</t>
-  </si>
-  <si>
-    <t>Rubric Grading</t>
-  </si>
-  <si>
-    <t>Formatting and presentation</t>
-  </si>
-  <si>
-    <t>Self-graded level</t>
-  </si>
-  <si>
-    <t>exceeds expectations</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Organization and flow</t>
-  </si>
-  <si>
-    <t>clearly meets expectations  / exceeds expectations</t>
-  </si>
-  <si>
-    <t>Technical content (intro, background)</t>
-  </si>
-  <si>
-    <t>Technical content (problem, design, results, testing)</t>
-  </si>
-  <si>
-    <t>clearly meets expectations</t>
-  </si>
-  <si>
-    <t>Plan for next semester</t>
-  </si>
-  <si>
-    <t>Impact on society and environment</t>
-  </si>
-  <si>
     <t>+/- 15V (TPS65131) boost quiescent current</t>
   </si>
   <si>
@@ -1048,6 +840,57 @@
   </si>
   <si>
     <t>+12V LDO quiescent draw (LDK320AM120R)</t>
+  </si>
+  <si>
+    <t>14 bits of data, but 16 bits total in the transaction sent in groups of 8 bits</t>
+  </si>
+  <si>
+    <t>Dead time from CS low to start of transaction</t>
+  </si>
+  <si>
+    <t>SCLK frequency</t>
+  </si>
+  <si>
+    <t>SCLK low time</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>SCLK high time</t>
+  </si>
+  <si>
+    <t>Output valid from SCLK low</t>
+  </si>
+  <si>
+    <t>CNVST pulse width high time</t>
+  </si>
+  <si>
+    <t>Equivalent bits from CS low to start of transaction</t>
+  </si>
+  <si>
+    <t>number of equivalent clock cycles, estimated</t>
+  </si>
+  <si>
+    <t>t_EN in datasheet</t>
+  </si>
+  <si>
+    <t>t_QUIET in datasheet</t>
+  </si>
+  <si>
+    <t>Equivalent bits from end to CS high</t>
+  </si>
+  <si>
+    <t>shared by all ADCs</t>
+  </si>
+  <si>
+    <t>Non-Inverting Gain Stage Tolerance Calculations</t>
+  </si>
+  <si>
+    <t>dB to V</t>
+  </si>
+  <si>
+    <t>ADC SPI Bandwidth (UNFINISHED CALCULATIONS)</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +903,7 @@
     <numFmt numFmtId="166" formatCode="##0.00E+0"/>
     <numFmt numFmtId="167" formatCode="##0.000E+0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1111,22 +954,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1462,7 +1289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1564,12 +1391,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1647,37 +1472,7 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3153,7 +2948,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>246766</xdr:colOff>
+      <xdr:colOff>246765</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>6262</xdr:rowOff>
     </xdr:to>
@@ -3318,6 +3113,55 @@
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>224852</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>131044</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA1B3E0-9A56-B293-A5C7-D88EFA5B79EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9368852" y="1948721"/>
+          <a:ext cx="5508886" cy="3503831"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3627,7 +3471,7 @@
   </sheetPr>
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0">
+    <sheetView zoomScale="91" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -3645,55 +3489,55 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64" t="s">
+      <c r="K3" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="F3" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>115</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
       <c r="G4" s="25"/>
-      <c r="K4" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="M4" s="67" t="s">
-        <v>113</v>
-      </c>
-      <c r="N4" s="68" t="s">
-        <v>114</v>
+      <c r="K4" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="M4" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="N4" s="66" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="77"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E5" s="16">
         <v>1.05</v>
@@ -3704,7 +3548,7 @@
       <c r="G5" s="26">
         <v>1.07</v>
       </c>
-      <c r="K5" s="69" t="str">
+      <c r="K5" s="67" t="str">
         <f>B4</f>
         <v>+5V</v>
       </c>
@@ -3716,15 +3560,15 @@
         <f>F15</f>
         <v>286.62175000000002</v>
       </c>
-      <c r="N5" s="70">
+      <c r="N5" s="68">
         <f>G15</f>
         <v>368.49974999999995</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="77"/>
+      <c r="B6" s="75"/>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E6" s="16">
         <v>90</v>
@@ -3735,7 +3579,7 @@
       <c r="G6" s="26">
         <v>110</v>
       </c>
-      <c r="K6" s="69" t="str">
+      <c r="K6" s="67" t="str">
         <f>B17</f>
         <v>+3V3</v>
       </c>
@@ -3747,15 +3591,15 @@
         <f t="shared" ref="M6:N6" si="0">F30</f>
         <v>11.328000000000001</v>
       </c>
-      <c r="N6" s="70">
+      <c r="N6" s="68">
         <f t="shared" si="0"/>
         <v>12.381999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="77"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="9" t="s">
-        <v>306</v>
+        <v>237</v>
       </c>
       <c r="E7" s="16">
         <v>0.5</v>
@@ -3766,7 +3610,7 @@
       <c r="G7" s="26">
         <v>0.72399999999999998</v>
       </c>
-      <c r="K7" s="69" t="str">
+      <c r="K7" s="67" t="str">
         <f>B32</f>
         <v>+12V</v>
       </c>
@@ -3778,15 +3622,15 @@
         <f t="shared" ref="M7:N7" si="1">F45</f>
         <v>36.329000000000008</v>
       </c>
-      <c r="N7" s="70">
+      <c r="N7" s="68">
         <f t="shared" si="1"/>
         <v>55.140999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="77"/>
+      <c r="B8" s="75"/>
       <c r="G8" s="26"/>
-      <c r="K8" s="69" t="str">
+      <c r="K8" s="67" t="str">
         <f>B47</f>
         <v>-12V</v>
       </c>
@@ -3798,15 +3642,15 @@
         <f t="shared" ref="M8:N8" si="2">F58</f>
         <v>10</v>
       </c>
-      <c r="N8" s="70">
+      <c r="N8" s="68">
         <f t="shared" si="2"/>
         <v>10.012</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="77"/>
+      <c r="B9" s="75"/>
       <c r="G9" s="26"/>
-      <c r="K9" s="69" t="str">
+      <c r="K9" s="67" t="str">
         <f>B60</f>
         <v>+5V_A</v>
       </c>
@@ -3818,21 +3662,21 @@
         <f>F65</f>
         <v>1.8599999999999999</v>
       </c>
-      <c r="N9" s="70">
+      <c r="N9" s="68">
         <f>G65</f>
         <v>2.37</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="77"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="28"/>
-      <c r="K10" s="71" t="str">
+      <c r="K10" s="69" t="str">
         <f>B67</f>
         <v>+1V8_A</v>
       </c>
@@ -3844,15 +3688,15 @@
         <f>F70</f>
         <v>1.98</v>
       </c>
-      <c r="N10" s="72">
+      <c r="N10" s="70">
         <f>G70</f>
         <v>2.7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="77"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="9" t="s">
-        <v>307</v>
+        <v>238</v>
       </c>
       <c r="E11" s="16">
         <f>E45*15/_RAIL_5V/EFF_12V_BOOST</f>
@@ -3868,9 +3712,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="77"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="9" t="s">
-        <v>308</v>
+        <v>239</v>
       </c>
       <c r="E12" s="16">
         <f>E58*15/_RAIL_5V/EFF_12V_BOOST</f>
@@ -3886,9 +3730,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="77"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E13" s="16">
         <f>E30</f>
@@ -3904,14 +3748,14 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="77"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="9"/>
       <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="78"/>
+      <c r="B15" s="76"/>
       <c r="C15" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="29">
@@ -3927,18 +3771,18 @@
         <v>368.49974999999995</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="65"/>
+      <c r="B16" s="63"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="76" t="s">
-        <v>122</v>
+      <c r="B17" s="74" t="s">
+        <v>119</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="24"/>
@@ -3946,9 +3790,9 @@
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="77"/>
+      <c r="B18" s="75"/>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E18" s="16">
         <f>3*0.00012</f>
@@ -3964,9 +3808,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="77"/>
+      <c r="B19" s="75"/>
       <c r="C19" t="s">
-        <v>312</v>
+        <v>243</v>
       </c>
       <c r="E19" s="16">
         <f>4*0.002</f>
@@ -3982,9 +3826,9 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="77"/>
+      <c r="B20" s="75"/>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E20" s="16">
         <f>24*3.3/100000*1000</f>
@@ -4000,9 +3844,9 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="77"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E21" s="16">
         <v>3.3</v>
@@ -4015,9 +3859,9 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="77"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E22" s="16">
         <v>0.05</v>
@@ -4030,9 +3874,9 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="77"/>
+      <c r="B23" s="75"/>
       <c r="C23" t="s">
-        <v>311</v>
+        <v>242</v>
       </c>
       <c r="E23" s="16">
         <v>6.0000000000000001E-3</v>
@@ -4045,17 +3889,17 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="77"/>
+      <c r="B24" s="75"/>
       <c r="G24" s="26"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="77"/>
+      <c r="B25" s="75"/>
       <c r="G25" s="26"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="77"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="27"/>
@@ -4063,9 +3907,9 @@
       <c r="G26" s="28"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="77"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E27" s="16">
         <f>E70</f>
@@ -4081,17 +3925,17 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="77"/>
+      <c r="B28" s="75"/>
       <c r="G28" s="26"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="77"/>
+      <c r="B29" s="75"/>
       <c r="G29" s="26"/>
     </row>
     <row r="30" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="78"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="29">
@@ -4108,14 +3952,14 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="65"/>
+      <c r="B31" s="63"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="76" t="s">
-        <v>118</v>
+      <c r="B32" s="74" t="s">
+        <v>115</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="24"/>
@@ -4123,9 +3967,9 @@
       <c r="G32" s="25"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="77"/>
+      <c r="B33" s="75"/>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E33" s="16">
         <v>0.6</v>
@@ -4138,9 +3982,9 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="77"/>
+      <c r="B34" s="75"/>
       <c r="C34" t="s">
-        <v>318</v>
+        <v>249</v>
       </c>
       <c r="E34" s="16">
         <f>8*3.2</f>
@@ -4155,22 +3999,22 @@
         <v>36.799999999999997</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>314</v>
+        <v>245</v>
       </c>
       <c r="L34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="N34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="77"/>
+      <c r="B35" s="75"/>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E35" s="16">
         <f>0.01*4</f>
@@ -4185,7 +4029,7 @@
         <v>0.3</v>
       </c>
       <c r="K35" t="s">
-        <v>315</v>
+        <v>246</v>
       </c>
       <c r="L35">
         <v>6</v>
@@ -4197,13 +4041,13 @@
         <v>9</v>
       </c>
       <c r="O35" t="s">
-        <v>317</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="77"/>
+      <c r="B36" s="75"/>
       <c r="C36" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="E36" s="16">
         <v>5</v>
@@ -4214,23 +4058,23 @@
       <c r="G36" s="26">
         <v>10</v>
       </c>
-      <c r="K36" s="73" t="s">
-        <v>316</v>
-      </c>
-      <c r="L36" s="74">
+      <c r="K36" s="71" t="s">
+        <v>247</v>
+      </c>
+      <c r="L36" s="72">
         <v>3.2</v>
       </c>
-      <c r="M36" s="74">
+      <c r="M36" s="72">
         <v>3.2</v>
       </c>
-      <c r="N36" s="75">
+      <c r="N36" s="73">
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="77"/>
+      <c r="B37" s="75"/>
       <c r="C37" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E37" s="16">
         <v>2</v>
@@ -4243,9 +4087,9 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="77"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="9" t="s">
-        <v>319</v>
+        <v>250</v>
       </c>
       <c r="E38" s="16">
         <v>7.0000000000000007E-2</v>
@@ -4258,18 +4102,18 @@
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="77"/>
+      <c r="B39" s="75"/>
       <c r="C39" s="9"/>
       <c r="G39" s="26"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B40" s="77"/>
+      <c r="B40" s="75"/>
       <c r="G40" s="26"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="77"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="27"/>
@@ -4277,9 +4121,9 @@
       <c r="G41" s="28"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B42" s="77"/>
+      <c r="B42" s="75"/>
       <c r="C42" s="9" t="s">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="E42" s="16">
         <v>0.748</v>
@@ -4292,9 +4136,9 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B43" s="77"/>
+      <c r="B43" s="75"/>
       <c r="C43" s="9" t="s">
-        <v>310</v>
+        <v>241</v>
       </c>
       <c r="E43" s="16">
         <f>E65</f>
@@ -4310,13 +4154,13 @@
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="77"/>
+      <c r="B44" s="75"/>
       <c r="G44" s="26"/>
     </row>
     <row r="45" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="78"/>
+      <c r="B45" s="76"/>
       <c r="C45" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="29">
@@ -4333,14 +4177,14 @@
       </c>
     </row>
     <row r="46" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="65"/>
+      <c r="B46" s="63"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B47" s="76" t="s">
-        <v>119</v>
+      <c r="B47" s="74" t="s">
+        <v>116</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="24"/>
@@ -4348,9 +4192,9 @@
       <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B48" s="77"/>
+      <c r="B48" s="75"/>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E48" s="16">
         <f>4*0.001</f>
@@ -4366,9 +4210,9 @@
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="77"/>
+      <c r="B49" s="75"/>
       <c r="C49" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="E49" s="16">
         <v>2.5</v>
@@ -4381,9 +4225,9 @@
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="77"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E50" s="16">
         <v>1.1879999999999999</v>
@@ -4396,22 +4240,22 @@
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="77"/>
+      <c r="B51" s="75"/>
       <c r="C51" s="9"/>
       <c r="G51" s="26"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="77"/>
+      <c r="B52" s="75"/>
       <c r="G52" s="26"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="77"/>
+      <c r="B53" s="75"/>
       <c r="G53" s="26"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="77"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="27"/>
@@ -4419,9 +4263,9 @@
       <c r="G54" s="28"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="77"/>
+      <c r="B55" s="75"/>
       <c r="C55" s="9" t="s">
-        <v>313</v>
+        <v>244</v>
       </c>
       <c r="E55" s="16">
         <v>6</v>
@@ -4434,17 +4278,17 @@
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="77"/>
+      <c r="B56" s="75"/>
       <c r="G56" s="26"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="77"/>
+      <c r="B57" s="75"/>
       <c r="G57" s="26"/>
     </row>
     <row r="58" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="78"/>
+      <c r="B58" s="76"/>
       <c r="C58" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D58" s="23"/>
       <c r="E58" s="29">
@@ -4461,14 +4305,14 @@
       </c>
     </row>
     <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="65"/>
+      <c r="B59" s="63"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="76" t="s">
-        <v>123</v>
+      <c r="B60" s="74" t="s">
+        <v>120</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="24"/>
@@ -4476,9 +4320,9 @@
       <c r="G60" s="25"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="77"/>
+      <c r="B61" s="75"/>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E61" s="16">
         <f>3*0.00004</f>
@@ -4494,9 +4338,9 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="77"/>
+      <c r="B62" s="75"/>
       <c r="C62" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E62" s="40">
         <v>1.1000000000000001</v>
@@ -4504,22 +4348,22 @@
       <c r="F62" s="40">
         <v>1.2</v>
       </c>
-      <c r="G62" s="63">
+      <c r="G62" s="61">
         <v>1.5</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="77"/>
+      <c r="B63" s="75"/>
       <c r="G63" s="26"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="77"/>
+      <c r="B64" s="75"/>
       <c r="G64" s="26"/>
     </row>
     <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="78"/>
+      <c r="B65" s="76"/>
       <c r="C65" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D65" s="23"/>
       <c r="E65" s="29">
@@ -4537,11 +4381,11 @@
     </row>
     <row r="66" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="76" t="s">
-        <v>126</v>
+      <c r="B67" s="74" t="s">
+        <v>123</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D67" s="20"/>
       <c r="E67" s="24"/>
@@ -4549,9 +4393,9 @@
       <c r="G67" s="25"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="77"/>
+      <c r="B68" s="75"/>
       <c r="C68" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E68" s="16">
         <f>3*0.0015</f>
@@ -4567,16 +4411,16 @@
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B69" s="77"/>
+      <c r="B69" s="75"/>
       <c r="C69" s="9"/>
       <c r="E69"/>
       <c r="F69"/>
       <c r="G69" s="32"/>
     </row>
     <row r="70" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="78"/>
+      <c r="B70" s="76"/>
       <c r="C70" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D70" s="23"/>
       <c r="E70" s="29">
@@ -4593,22 +4437,22 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B71" s="65"/>
+      <c r="B71" s="63"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" s="65"/>
+      <c r="B72" s="63"/>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B74" s="65"/>
+      <c r="B74" s="63"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B75" s="65"/>
+      <c r="B75" s="63"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B76" s="65"/>
+      <c r="B76" s="63"/>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B77" s="65"/>
+      <c r="B77" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4620,7 +4464,7 @@
     <mergeCell ref="B60:B65"/>
   </mergeCells>
   <conditionalFormatting sqref="E15:G15">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>499.99</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4628,124 +4472,6 @@
   <pageSetup scale="46" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96BC64E-6859-4D78-886E-3CFB87C1F7CA}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <f>10^(B4/20)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>-3</v>
-      </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C12" si="0">10^(B5/20)</f>
-        <v>0.70794578438413791</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>-6</v>
-      </c>
-      <c r="C6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.50118723362727224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>-10</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31622776601683794</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>-20</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>-30</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="0"/>
-        <v>3.1622776601683784E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>-40</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>-50</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="0"/>
-        <v>3.1622776601683764E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>-60</v>
-      </c>
-      <c r="C12" s="4">
-        <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4757,7 +4483,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4787,7 +4513,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>27</v>
@@ -4798,7 +4524,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>-27</v>
@@ -4809,7 +4535,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -4820,7 +4546,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -4831,7 +4557,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -4842,7 +4568,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -4851,12 +4577,12 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>-0.3</v>
@@ -4865,7 +4591,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -4879,7 +4605,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -4895,7 +4621,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>3.3</v>
@@ -4906,7 +4632,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4917,7 +4643,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <f>(B15-B16)/(B6*0.001)</f>
@@ -4927,12 +4653,12 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <f>(B15-B16)/(B7*0.001)</f>
@@ -4945,7 +4671,7 @@
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="56">
         <v>470</v>
@@ -4956,7 +4682,7 @@
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="54">
         <v>10</v>
@@ -4967,7 +4693,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <f>(B15+B13)+B12/1000*B22</f>
@@ -4979,7 +4705,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <f>(B16-B13)-B12/1000*B22</f>
@@ -4991,7 +4717,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26">
         <f>B15/(B22+B23)*1000</f>
@@ -5003,19 +4729,19 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28">
         <f>B22*B12*B12/1000000</f>
         <v>7.34375</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="4">
         <f>SQRT(0.5/B22)*1000</f>
@@ -5027,7 +4753,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="52">
         <f>B15+B13+B29/1000*B22</f>
@@ -5039,7 +4765,7 @@
     </row>
     <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="54">
         <f>B16-B13-B29/1000*B22</f>
@@ -5051,7 +4777,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -5068,7 +4794,7 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -5099,7 +4825,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -5175,7 +4901,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5187,10 +4913,10 @@
         <v>2.5497289999999999E-2</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -5204,7 +4930,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -5264,7 +4990,7 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -5289,7 +5015,7 @@
         <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -5304,7 +5030,7 @@
         <v>21</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -5329,7 +5055,7 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G16" s="6">
         <f>5/G5*1000</f>
@@ -5353,29 +5079,29 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3">
         <f>B17/B12</f>
         <v>0.28044393432544817</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" s="3">
         <f>B17/G13</f>
         <v>2.6965762915908478</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
         <v>5</v>
@@ -5399,7 +5125,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G22">
         <v>3</v>
@@ -5436,7 +5162,7 @@
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -5447,7 +5173,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B25" s="4">
         <f>(B24-1.76)/6.02</f>
@@ -5483,27 +5209,27 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H27">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="I27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H28">
         <v>8896.4431999999997</v>
       </c>
       <c r="I28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -5528,12 +5254,12 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B31" s="4">
         <f>(B30-1.76)/6.02</f>
@@ -5557,23 +5283,23 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5591,7 +5317,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5605,23 +5331,23 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -5629,7 +5355,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -5637,42 +5363,42 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <f>C3/2^C4</f>
         <v>1.220703125E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="79" t="s">
-        <v>107</v>
+      <c r="A8" s="77" t="s">
+        <v>104</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" s="35">
         <v>1E-3</v>
@@ -5700,9 +5426,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
+      <c r="A9" s="78"/>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C9" s="36">
         <v>1E-3</v>
@@ -5723,12 +5449,12 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="80"/>
+      <c r="A10" s="78"/>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="16">
         <v>40</v>
@@ -5744,12 +5470,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="81"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="18">
         <f>1+(D8+D10)/F9</f>
@@ -5768,11 +5494,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="82" t="s">
-        <v>108</v>
+      <c r="A12" s="80" t="s">
+        <v>105</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C12" s="35">
         <v>1E-3</v>
@@ -5800,9 +5526,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
+      <c r="A13" s="81"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C13" s="36">
         <v>1E-3</v>
@@ -5824,12 +5550,12 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
+      <c r="A14" s="81"/>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="16">
         <v>40</v>
@@ -5845,12 +5571,12 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="84"/>
+      <c r="A15" s="82"/>
       <c r="B15" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="18">
         <f>1+(D12+D14)/F13</f>
@@ -5869,11 +5595,11 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
-        <v>109</v>
+      <c r="A16" s="83" t="s">
+        <v>106</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C16" s="35">
         <v>1E-3</v>
@@ -5901,9 +5627,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="86"/>
+      <c r="A17" s="84"/>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C17" s="36">
         <v>1E-3</v>
@@ -5925,12 +5651,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="86"/>
+      <c r="A18" s="84"/>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18" s="16">
         <v>40</v>
@@ -5946,12 +5672,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="87"/>
+      <c r="A19" s="85"/>
       <c r="B19" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="18">
         <f>1+(D16+D18)/D17</f>
@@ -5970,11 +5696,11 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="88" t="s">
-        <v>110</v>
+      <c r="A20" s="86" t="s">
+        <v>107</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" s="35">
         <v>1E-3</v>
@@ -6002,9 +5728,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="89"/>
+      <c r="A21" s="87"/>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" s="36">
         <v>1E-3</v>
@@ -6026,12 +5752,12 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="89"/>
+      <c r="A22" s="87"/>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16">
         <v>40</v>
@@ -6047,12 +5773,12 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="90"/>
+      <c r="A23" s="88"/>
       <c r="B23" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D23" s="18">
         <f>1+(D20+D22)/F21</f>
@@ -6091,7 +5817,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6099,14 +5825,14 @@
     <col min="1" max="1" width="35.109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.21875" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="9" max="9" width="43.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -6137,35 +5863,35 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5">
         <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G5">
         <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -6174,10 +5900,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G6">
         <v>-15</v>
@@ -6188,7 +5914,7 @@
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7">
         <v>1.2130000000000001</v>
@@ -6197,10 +5923,10 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G7">
         <v>1.2130000000000001</v>
@@ -6211,70 +5937,70 @@
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B8" s="45">
         <v>47.5</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G8" s="45">
         <v>47.5</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B9">
         <f>B8*(B6/B7-1)</f>
         <v>539.88664468260504</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G9">
         <f>-1*G8*G6/G7</f>
         <v>587.38664468260504</v>
       </c>
       <c r="H9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="45">
         <v>536</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G11" s="45">
         <v>576</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B12">
         <f>(1+B11/B8)*B7</f>
@@ -6284,7 +6010,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G12">
         <f>-G11/G8*G7</f>
@@ -6296,15 +6022,15 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -6313,7 +6039,7 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G23">
         <v>5</v>
@@ -6324,133 +6050,133 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B24">
         <v>0.08</v>
       </c>
       <c r="C24" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" t="s">
         <v>179</v>
-      </c>
-      <c r="D24" t="s">
-        <v>180</v>
-      </c>
-      <c r="F24" t="s">
-        <v>182</v>
       </c>
       <c r="G24">
         <v>0.01</v>
       </c>
       <c r="H24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B25">
         <f>B6/(B23*0.64)*B24</f>
         <v>0.375</v>
       </c>
       <c r="C25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F25" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G25">
         <f>(G23-G6)/(G23*0.64)*G24</f>
         <v>6.25E-2</v>
       </c>
       <c r="H25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B26">
         <f>0.2*B25</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G26">
         <f>0.2*G25</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="H26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B27">
         <v>1.25</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G27">
         <v>1.25</v>
       </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B28" s="47">
         <f>B23*(B6-B23)/(B26*B27*B6)</f>
         <v>35.55555555555555</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F28" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G28" s="48">
         <f>G23*G6/(G26*G27*(G6-G23))</f>
         <v>240</v>
       </c>
       <c r="H28" s="48" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I28" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B32">
         <v>5.0000000000000001E-3</v>
@@ -6459,7 +6185,7 @@
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G32">
         <v>5.0000000000000001E-3</v>
@@ -6470,29 +6196,29 @@
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B33" s="49">
         <f>B24*(B6-B23)/(B27*B32*B6)</f>
         <v>8.5333333333333332</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G33" s="45">
         <f>G24*G6/(G27*G32*(G6-G23))</f>
         <v>1.2</v>
       </c>
       <c r="H33" s="46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B34">
         <v>0.01</v>
@@ -6501,7 +6227,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G34">
         <v>0.01</v>
@@ -6512,7 +6238,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B35">
         <f>B24*B34</f>
@@ -6522,7 +6248,7 @@
         <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G35">
         <f>G24*G34</f>
@@ -6534,52 +6260,52 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B39" s="50">
         <f>0.0000068/(B11*1000)</f>
         <v>1.2686567164179104E-11</v>
       </c>
       <c r="C39" t="s">
+        <v>198</v>
+      </c>
+      <c r="F39" t="s">
         <v>201</v>
-      </c>
-      <c r="F39" t="s">
-        <v>204</v>
       </c>
       <c r="G39" s="50">
         <f>0.0000075/(G11*1000)</f>
         <v>1.3020833333333334E-11</v>
       </c>
       <c r="H39" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B40">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F40" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G40">
         <v>13</v>
       </c>
       <c r="H40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -6596,8 +6322,8 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6609,7 +6335,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6617,16 +6343,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>3</v>
@@ -6636,15 +6362,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
-        <v>229</v>
+      <c r="A4" s="57" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" s="59">
+        <v>218</v>
+      </c>
+      <c r="B5" s="58">
         <v>0.01</v>
       </c>
       <c r="C5">
@@ -6659,14 +6385,14 @@
         <v>541.36</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>226</v>
-      </c>
-      <c r="B6" s="59">
+        <v>219</v>
+      </c>
+      <c r="B6" s="58">
         <v>0.01</v>
       </c>
       <c r="C6">
@@ -6681,15 +6407,15 @@
         <v>49.187000000000005</v>
       </c>
       <c r="F6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>1.2</v>
@@ -6706,20 +6432,20 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="45">
         <f>C7*(C5/E6+1)</f>
         <v>14.145859678370298</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="59">
         <f>D7*(D5/D6+1)</f>
         <v>14.563472279260779</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="59">
         <f>E7*(E5/C6+1)</f>
         <v>14.979920871963994</v>
       </c>
@@ -6728,15 +6454,15 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="58" t="s">
-        <v>230</v>
+      <c r="A10" s="57" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" s="59">
+        <v>224</v>
+      </c>
+      <c r="B11" s="58">
         <v>0.01</v>
       </c>
       <c r="C11">
@@ -6751,14 +6477,14 @@
         <v>581.76</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="59">
+        <v>225</v>
+      </c>
+      <c r="B12" s="58">
         <v>0.01</v>
       </c>
       <c r="C12">
@@ -6773,15 +6499,15 @@
         <v>49.187000000000005</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>1.2</v>
@@ -6798,20 +6524,20 @@
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="45">
         <f>-E13*E11/C12</f>
         <v>-14.781407504200113</v>
       </c>
-      <c r="D14" s="60">
+      <c r="D14" s="59">
         <f>-D13*D11/D12</f>
         <v>-14.346776180698154</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="59">
         <f>-C13*C11/E12</f>
         <v>-13.911968609591964</v>
       </c>
@@ -6820,16 +6546,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="58" t="s">
-        <v>233</v>
+      <c r="A16" s="57" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>0.7</v>
@@ -6846,7 +6572,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C18">
         <f>12+C17</f>
@@ -6864,36 +6590,36 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="59">
+        <v>232</v>
+      </c>
+      <c r="C19" s="58">
         <v>-0.03</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="58">
         <v>0</v>
       </c>
-      <c r="E19" s="59">
+      <c r="E19" s="58">
         <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C20" s="45">
         <f>12*(1+C19)</f>
         <v>11.64</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="59">
         <f>12*(1+D19)</f>
         <v>12</v>
       </c>
-      <c r="E20" s="60">
+      <c r="E20" s="59">
         <f>12*(1+E19)</f>
         <v>12.36</v>
       </c>
@@ -6902,16 +6628,16 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="58" t="s">
-        <v>236</v>
+      <c r="A22" s="57" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23">
         <v>1.7</v>
@@ -6928,7 +6654,7 @@
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C24">
         <f>-12-C23</f>
@@ -6946,37 +6672,37 @@
         <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C25" s="45">
         <v>-11.4</v>
       </c>
-      <c r="D25" s="60">
+      <c r="D25" s="59">
         <v>-12</v>
       </c>
-      <c r="E25" s="60">
+      <c r="E25" s="59">
         <v>-12.6</v>
       </c>
       <c r="F25" s="46" t="s">
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="58" t="s">
-        <v>241</v>
+      <c r="A27" s="57" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C28">
         <v>0.35</v>
@@ -6993,7 +6719,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C29">
         <f>1.8+C28</f>
@@ -7011,39 +6737,39 @@
         <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="61">
+        <v>61</v>
+      </c>
+      <c r="C30" s="60">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="D30" s="59">
+      <c r="D30" s="58">
         <v>0</v>
       </c>
-      <c r="E30" s="61">
+      <c r="E30" s="60">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C31" s="45">
         <f>1.8*(1+C30)</f>
         <v>1.7729999999999999</v>
       </c>
-      <c r="D31" s="60">
+      <c r="D31" s="59">
         <f>1.8*(1+D30)</f>
         <v>1.8</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <f>1.8*(1+E30)</f>
         <v>1.827</v>
       </c>
@@ -7065,7 +6791,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7077,7 +6803,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -7085,16 +6811,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>3</v>
@@ -7105,10 +6831,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="16">
         <f>3*0.00004</f>
@@ -7128,10 +6854,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="16">
         <v>1</v>
@@ -7146,15 +6872,15 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="16">
         <f>C4+C5</f>
@@ -7179,10 +6905,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="16">
         <v>11.9</v>
@@ -7197,15 +6923,15 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="16">
         <v>4.9950000000000001</v>
@@ -7227,7 +6953,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C11" s="16">
         <f>C8-E9</f>
@@ -7247,7 +6973,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C12" s="37">
         <f>C11/E6</f>
@@ -7262,7 +6988,7 @@
         <v>7.1041475022997247</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -7272,10 +6998,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="40">
@@ -7284,10 +7010,10 @@
       </c>
       <c r="E14" s="16"/>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7297,7 +7023,7 @@
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="41" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B16" s="42">
         <v>0.01</v>
@@ -7314,12 +7040,12 @@
         <v>4.2622</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C17" s="31">
         <f>C11/E16-E4</f>
@@ -7337,7 +7063,7 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -7352,25 +7078,43 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -7383,718 +7127,436 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>30</v>
       </c>
       <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5">
+        <f>1/(B4*1000000)</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="G5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>251</v>
+      </c>
+      <c r="G7" t="s">
+        <v>257</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>252</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+      <c r="D9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B10">
+        <f>B9*0.000000001/B5</f>
+        <v>0.2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>255</v>
+      </c>
+      <c r="D11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12">
+        <f>B11*0.000000001/B5</f>
+        <v>0.2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(B7:B12)*B5</f>
+        <v>2.0700000000000001E-6</v>
+      </c>
+      <c r="C16" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="5">
-        <f>1/(B9*1000000)</f>
-        <v>2.4999999999999999E-8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="5">
-        <f>SUM(B4:B7)*B10</f>
-        <v>7.7499999999999999E-7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="5">
-        <f>1/B12</f>
-        <v>1290322.5806451612</v>
-      </c>
-      <c r="D13" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17">
-        <v>56000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
+        <v>35</v>
+      </c>
+      <c r="B17" s="5">
+        <f>1/B16</f>
+        <v>483091.78743961349</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19">
-        <v>100</v>
-      </c>
-      <c r="C19" t="s">
-        <v>72</v>
+      <c r="A19" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>56000</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B22">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28">
+        <f>(B25+B26)*(B23*B22+B21*B20)/1000000</f>
+        <v>8.9920000000000009</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B25">
-        <f>(B22+B23)*(B20*B19+B18*B17)/1000000</f>
-        <v>8.9920000000000009</v>
-      </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29">
+      <c r="B32">
         <v>24</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31">
-        <v>100000</v>
-      </c>
-      <c r="C31" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B33">
-        <f>B31*B29/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34">
+        <v>100000</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36">
+        <f>B34*B32/1000000</f>
         <v>2.4</v>
       </c>
-      <c r="C33" t="s">
-        <v>76</v>
+      <c r="C36" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4773A798-633B-4D8D-9FC8-9ECE55BCD182}">
-  <dimension ref="A1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96BC64E-6859-4D78-886E-3CFB87C1F7CA}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>245</v>
-      </c>
-      <c r="B4" t="s">
-        <v>260</v>
-      </c>
-      <c r="F4" t="s">
-        <v>244</v>
-      </c>
-      <c r="G4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" t="s">
-        <v>260</v>
-      </c>
-      <c r="F5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B6" t="s">
-        <v>260</v>
-      </c>
-      <c r="F6" t="s">
-        <v>283</v>
-      </c>
-      <c r="G6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>248</v>
-      </c>
-      <c r="B7" t="s">
-        <v>260</v>
-      </c>
-      <c r="F7" t="s">
-        <v>284</v>
-      </c>
-      <c r="G7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>249</v>
-      </c>
-      <c r="B8" t="s">
-        <v>260</v>
-      </c>
-      <c r="F8" t="s">
-        <v>246</v>
-      </c>
-      <c r="G8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>250</v>
-      </c>
-      <c r="B9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F9" t="s">
-        <v>247</v>
-      </c>
-      <c r="G9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>251</v>
-      </c>
-      <c r="B10" t="s">
-        <v>260</v>
-      </c>
-      <c r="F10" t="s">
-        <v>248</v>
-      </c>
-      <c r="G10" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>252</v>
-      </c>
-      <c r="B11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F11" t="s">
-        <v>249</v>
-      </c>
-      <c r="G11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>253</v>
-      </c>
-      <c r="B12" t="s">
-        <v>260</v>
-      </c>
-      <c r="F12" t="s">
-        <v>250</v>
-      </c>
-      <c r="G12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>260</v>
-      </c>
-      <c r="C13" s="62" t="s">
-        <v>261</v>
-      </c>
-      <c r="F13" t="s">
-        <v>285</v>
-      </c>
-      <c r="G13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" t="s">
-        <v>260</v>
-      </c>
-      <c r="F14" t="s">
-        <v>252</v>
-      </c>
-      <c r="G14" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" t="s">
-        <v>260</v>
-      </c>
-      <c r="F15" t="s">
-        <v>286</v>
-      </c>
-      <c r="G15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16" t="s">
-        <v>260</v>
-      </c>
-      <c r="F16" t="s">
-        <v>287</v>
-      </c>
-      <c r="G16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F17" t="s">
-        <v>288</v>
-      </c>
-      <c r="G17" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F18" t="s">
-        <v>289</v>
-      </c>
-      <c r="G18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>264</v>
-      </c>
-      <c r="B19" t="s">
-        <v>260</v>
-      </c>
-      <c r="C19" t="s">
-        <v>277</v>
-      </c>
-      <c r="F19" t="s">
-        <v>253</v>
-      </c>
-      <c r="G19" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>265</v>
-      </c>
-      <c r="B20" t="s">
-        <v>260</v>
-      </c>
-      <c r="F20" t="s">
-        <v>257</v>
-      </c>
-      <c r="G20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="B21" t="s">
-        <v>260</v>
-      </c>
-      <c r="F21" t="s">
-        <v>290</v>
-      </c>
-      <c r="G21" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>268</v>
-      </c>
-      <c r="B23" t="s">
-        <v>260</v>
-      </c>
-      <c r="C23" t="s">
-        <v>278</v>
-      </c>
-      <c r="F23" t="s">
-        <v>292</v>
-      </c>
-      <c r="G23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>269</v>
-      </c>
-      <c r="B24" t="s">
-        <v>260</v>
-      </c>
-      <c r="F24" t="s">
-        <v>293</v>
-      </c>
-      <c r="G24" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>270</v>
-      </c>
-      <c r="B25" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>271</v>
-      </c>
-      <c r="B26" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>272</v>
-      </c>
-      <c r="B27" t="s">
-        <v>260</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>274</v>
-      </c>
-      <c r="B28" t="s">
-        <v>260</v>
-      </c>
-      <c r="F28" t="s">
-        <v>295</v>
-      </c>
-      <c r="G28" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>273</v>
-      </c>
-      <c r="B29" t="s">
-        <v>260</v>
-      </c>
-      <c r="F29" t="s">
-        <v>298</v>
-      </c>
-      <c r="G29" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>275</v>
-      </c>
-      <c r="B30" t="s">
-        <v>260</v>
-      </c>
-      <c r="F30" t="s">
-        <v>299</v>
-      </c>
-      <c r="G30" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>276</v>
-      </c>
-      <c r="B31" t="s">
-        <v>260</v>
-      </c>
-      <c r="F31" t="s">
-        <v>301</v>
-      </c>
-      <c r="G31" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>291</v>
-      </c>
-      <c r="B32" t="s">
-        <v>260</v>
-      </c>
-      <c r="F32" t="s">
-        <v>302</v>
-      </c>
-      <c r="G32" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F33" t="s">
-        <v>304</v>
-      </c>
-      <c r="G33" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" t="s">
-        <v>305</v>
-      </c>
-      <c r="G34" t="s">
-        <v>303</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <f>10^(B4/20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>-3</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C12" si="0">10^(B5/20)</f>
+        <v>0.70794578438413791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>-6</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.50118723362727224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>-10</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>-20</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>-30</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>3.1622776601683784E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>-40</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>-50</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>3.1622776601683764E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>-60</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B159">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>